<commit_message>
started refactoring of calc_correlations_with_areas_approach
</commit_message>
<xml_diff>
--- a/my_project/corr_search_res/correlation_sectors_approach_data.xlsx
+++ b/my_project/corr_search_res/correlation_sectors_approach_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N93"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,50 +456,35 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>avg_distance</t>
+          <t>store_density_3km</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>sum_population_metric</t>
+          <t>population_density_3km</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>avg_population_metric</t>
+          <t>population_metric_sum_3km</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>store_density_3km</t>
+          <t>population_metric_avg_3km</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>population_density_3km</t>
+          <t>population_uniformity_3km</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>population_metric_sum_3km</t>
+          <t>population_store_ratio_3km</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>population_metric_avg_3km</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>population_uniformity_3km</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>population_store_ratio_3km</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>pop_metric_store_ratio_3km</t>
         </is>
@@ -521,34 +506,25 @@
         <v>2.182984967003582</v>
       </c>
       <c r="E2" t="n">
-        <v>1.555884063417384</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
-        <v>412.5509236128018</v>
+        <v>165</v>
       </c>
       <c r="G2" t="n">
-        <v>2.266763316553856</v>
+        <v>374.1354943038655</v>
       </c>
       <c r="H2" t="n">
-        <v>51</v>
+        <v>2.267487844265851</v>
       </c>
       <c r="I2" t="n">
-        <v>1591</v>
+        <v>50.17100037018368</v>
       </c>
       <c r="J2" t="n">
-        <v>3317.172024221586</v>
+        <v>23.57142857142857</v>
       </c>
       <c r="K2" t="n">
-        <v>2.084960417486855</v>
-      </c>
-      <c r="L2" t="n">
-        <v>378.515501317934</v>
-      </c>
-      <c r="M2" t="n">
-        <v>31.19607843137255</v>
-      </c>
-      <c r="N2" t="n">
-        <v>65.04258871022718</v>
+        <v>53.44792775769507</v>
       </c>
     </row>
     <row r="3">
@@ -567,34 +543,25 @@
         <v>2.636888906983799</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5269650585014904</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
-        <v>170.4104773369512</v>
+        <v>124</v>
       </c>
       <c r="G3" t="n">
-        <v>2.334390100506181</v>
+        <v>295.4401416798368</v>
       </c>
       <c r="H3" t="n">
-        <v>51</v>
+        <v>2.382581787740619</v>
       </c>
       <c r="I3" t="n">
-        <v>652</v>
+        <v>20.17507514430831</v>
       </c>
       <c r="J3" t="n">
-        <v>1457.837841431452</v>
+        <v>13.77777777777778</v>
       </c>
       <c r="K3" t="n">
-        <v>2.235947609557443</v>
-      </c>
-      <c r="L3" t="n">
-        <v>237.6524758661601</v>
-      </c>
-      <c r="M3" t="n">
-        <v>12.7843137254902</v>
-      </c>
-      <c r="N3" t="n">
-        <v>28.58505571434221</v>
+        <v>32.82668240887075</v>
       </c>
     </row>
     <row r="4">
@@ -613,34 +580,25 @@
         <v>2.503790683057181</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3756375651490761</v>
+        <v>18</v>
       </c>
       <c r="F4" t="n">
-        <v>93.23616690654964</v>
+        <v>174</v>
       </c>
       <c r="G4" t="n">
-        <v>2.51989640287972</v>
+        <v>426.0018146215393</v>
       </c>
       <c r="H4" t="n">
-        <v>87</v>
+        <v>2.448286290928387</v>
       </c>
       <c r="I4" t="n">
-        <v>1066</v>
+        <v>14.72124807682166</v>
       </c>
       <c r="J4" t="n">
-        <v>2503.576284877788</v>
+        <v>9.666666666666666</v>
       </c>
       <c r="K4" t="n">
-        <v>2.348570623712746</v>
-      </c>
-      <c r="L4" t="n">
-        <v>246.4847351622994</v>
-      </c>
-      <c r="M4" t="n">
-        <v>12.25287356321839</v>
-      </c>
-      <c r="N4" t="n">
-        <v>28.77673890664124</v>
+        <v>23.66676747897441</v>
       </c>
     </row>
     <row r="5">
@@ -659,34 +617,25 @@
         <v>2.376576957056512</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6922199983784504</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>256.0777932364393</v>
+        <v>178</v>
       </c>
       <c r="G5" t="n">
-        <v>2.081933278345035</v>
+        <v>373.2706681672649</v>
       </c>
       <c r="H5" t="n">
-        <v>69</v>
+        <v>2.097026225658792</v>
       </c>
       <c r="I5" t="n">
-        <v>1505</v>
+        <v>55.53857474474825</v>
       </c>
       <c r="J5" t="n">
-        <v>3022.909355932684</v>
+        <v>25.42857142857143</v>
       </c>
       <c r="K5" t="n">
-        <v>2.008577645137996</v>
-      </c>
-      <c r="L5" t="n">
-        <v>458.5239756844566</v>
-      </c>
-      <c r="M5" t="n">
-        <v>21.81159420289855</v>
-      </c>
-      <c r="N5" t="n">
-        <v>43.81028052076354</v>
+        <v>53.32438116675213</v>
       </c>
     </row>
     <row r="6">
@@ -705,34 +654,25 @@
         <v>2.340840549812332</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7015359270070849</v>
+        <v>8</v>
       </c>
       <c r="F6" t="n">
-        <v>247.252027713374</v>
+        <v>134</v>
       </c>
       <c r="G6" t="n">
-        <v>2.49749522942802</v>
+        <v>328.9899425302744</v>
       </c>
       <c r="H6" t="n">
-        <v>33</v>
+        <v>2.455148824852794</v>
       </c>
       <c r="I6" t="n">
-        <v>458</v>
+        <v>61.11243330291155</v>
       </c>
       <c r="J6" t="n">
-        <v>1130.806890553545</v>
+        <v>16.75</v>
       </c>
       <c r="K6" t="n">
-        <v>2.469010678064508</v>
-      </c>
-      <c r="L6" t="n">
-        <v>255.7848002421889</v>
-      </c>
-      <c r="M6" t="n">
-        <v>13.87878787878788</v>
-      </c>
-      <c r="N6" t="n">
-        <v>34.26687547131954</v>
+        <v>41.12374281628431</v>
       </c>
     </row>
     <row r="7">
@@ -751,34 +691,25 @@
         <v>2.15956719323362</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7546067567675219</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
-        <v>893.5605132939996</v>
+        <v>506</v>
       </c>
       <c r="G7" t="n">
-        <v>1.889134277577166</v>
+        <v>971.9453740898773</v>
       </c>
       <c r="H7" t="n">
-        <v>62</v>
+        <v>1.920840660256675</v>
       </c>
       <c r="I7" t="n">
-        <v>2368</v>
+        <v>91.28386487901908</v>
       </c>
       <c r="J7" t="n">
-        <v>4703.246273588045</v>
+        <v>63.25</v>
       </c>
       <c r="K7" t="n">
-        <v>1.986168189859816</v>
-      </c>
-      <c r="L7" t="n">
-        <v>348.4471835698485</v>
-      </c>
-      <c r="M7" t="n">
-        <v>38.19354838709678</v>
-      </c>
-      <c r="N7" t="n">
-        <v>75.85881086432332</v>
+        <v>121.4931717612347</v>
       </c>
     </row>
     <row r="8">
@@ -797,34 +728,25 @@
         <v>2.405687786672777</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4423684469186583</v>
+        <v>11</v>
       </c>
       <c r="F8" t="n">
-        <v>167.856999565512</v>
+        <v>149</v>
       </c>
       <c r="G8" t="n">
-        <v>2.268337831966379</v>
+        <v>350.9968118056257</v>
       </c>
       <c r="H8" t="n">
-        <v>55</v>
+        <v>2.355683300708897</v>
       </c>
       <c r="I8" t="n">
-        <v>775</v>
+        <v>23.31617888878278</v>
       </c>
       <c r="J8" t="n">
-        <v>1761.259392153236</v>
+        <v>13.54545454545454</v>
       </c>
       <c r="K8" t="n">
-        <v>2.272592764068692</v>
-      </c>
-      <c r="L8" t="n">
-        <v>362.9301697632641</v>
-      </c>
-      <c r="M8" t="n">
-        <v>14.09090909090909</v>
-      </c>
-      <c r="N8" t="n">
-        <v>32.02289803914975</v>
+        <v>31.9088010732387</v>
       </c>
     </row>
     <row r="9">
@@ -843,34 +765,25 @@
         <v>2.3654879848909</v>
       </c>
       <c r="E9" t="n">
-        <v>1.591910975164802</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
-        <v>136.7866105560617</v>
+        <v>18</v>
       </c>
       <c r="G9" t="n">
-        <v>2.137290789938464</v>
+        <v>39.07709333091777</v>
       </c>
       <c r="H9" t="n">
+        <v>2.170949629495432</v>
+      </c>
+      <c r="I9" t="n">
+        <v>9.049033018207503</v>
+      </c>
+      <c r="J9" t="n">
         <v>6</v>
       </c>
-      <c r="I9" t="n">
-        <v>132</v>
-      </c>
-      <c r="J9" t="n">
-        <v>283.4984150568557</v>
-      </c>
       <c r="K9" t="n">
-        <v>2.14771526558224</v>
-      </c>
-      <c r="L9" t="n">
-        <v>71.69817703538827</v>
-      </c>
-      <c r="M9" t="n">
-        <v>22</v>
-      </c>
-      <c r="N9" t="n">
-        <v>47.24973584280929</v>
+        <v>13.02569777697259</v>
       </c>
     </row>
     <row r="10">
@@ -889,34 +802,25 @@
         <v>2.781108835729466</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5076407256295041</v>
+        <v>14</v>
       </c>
       <c r="F10" t="n">
-        <v>308.9766509245752</v>
+        <v>308</v>
       </c>
       <c r="G10" t="n">
-        <v>2.101881979078743</v>
+        <v>643.5342708232462</v>
       </c>
       <c r="H10" t="n">
-        <v>76</v>
+        <v>2.089396983192358</v>
       </c>
       <c r="I10" t="n">
-        <v>1969</v>
+        <v>43.69869132356197</v>
       </c>
       <c r="J10" t="n">
-        <v>3909.280726953545</v>
+        <v>22</v>
       </c>
       <c r="K10" t="n">
-        <v>1.985414284892608</v>
-      </c>
-      <c r="L10" t="n">
-        <v>373.0592806032815</v>
-      </c>
-      <c r="M10" t="n">
-        <v>25.90789473684211</v>
-      </c>
-      <c r="N10" t="n">
-        <v>51.43790430202033</v>
+        <v>45.96673363023187</v>
       </c>
     </row>
     <row r="11">
@@ -935,34 +839,25 @@
         <v>2.62705846400099</v>
       </c>
       <c r="E11" t="n">
-        <v>1.085155246051337</v>
+        <v>16</v>
       </c>
       <c r="F11" t="n">
-        <v>762.0423288412494</v>
+        <v>253</v>
       </c>
       <c r="G11" t="n">
-        <v>2.140568339441712</v>
+        <v>544.4324451584469</v>
       </c>
       <c r="H11" t="n">
-        <v>101</v>
+        <v>2.151906897859474</v>
       </c>
       <c r="I11" t="n">
-        <v>1659</v>
+        <v>49.04358452225105</v>
       </c>
       <c r="J11" t="n">
-        <v>3448.46021022019</v>
+        <v>15.8125</v>
       </c>
       <c r="K11" t="n">
-        <v>2.078637860289446</v>
-      </c>
-      <c r="L11" t="n">
-        <v>216.6011138837769</v>
-      </c>
-      <c r="M11" t="n">
-        <v>16.42574257425743</v>
-      </c>
-      <c r="N11" t="n">
-        <v>34.1431703982197</v>
+        <v>34.02702782240293</v>
       </c>
     </row>
     <row r="12">
@@ -981,34 +876,25 @@
         <v>2.182414652434554</v>
       </c>
       <c r="E12" t="n">
-        <v>1.603658218748081</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
-        <v>605.0084523918839</v>
+        <v>100</v>
       </c>
       <c r="G12" t="n">
-        <v>1.957956156608039</v>
+        <v>228.7929692573303</v>
       </c>
       <c r="H12" t="n">
-        <v>46</v>
+        <v>2.287929692573303</v>
       </c>
       <c r="I12" t="n">
-        <v>769</v>
+        <v>30.64313677998844</v>
       </c>
       <c r="J12" t="n">
-        <v>1594.731903135436</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="K12" t="n">
-        <v>2.073773606157914</v>
-      </c>
-      <c r="L12" t="n">
-        <v>226.4987052541661</v>
-      </c>
-      <c r="M12" t="n">
-        <v>16.71739130434782</v>
-      </c>
-      <c r="N12" t="n">
-        <v>34.66808485077034</v>
+        <v>25.42144102859226</v>
       </c>
     </row>
     <row r="13">
@@ -1027,34 +913,25 @@
         <v>2.582744965691277</v>
       </c>
       <c r="E13" t="n">
-        <v>1.490088876560463</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
-        <v>339.5098274463416</v>
+        <v>123</v>
       </c>
       <c r="G13" t="n">
-        <v>2.325409777029737</v>
+        <v>288.6648792345596</v>
       </c>
       <c r="H13" t="n">
-        <v>70</v>
+        <v>2.346868936866338</v>
       </c>
       <c r="I13" t="n">
-        <v>799</v>
+        <v>27.39309080912003</v>
       </c>
       <c r="J13" t="n">
-        <v>1862.874005209825</v>
+        <v>15.375</v>
       </c>
       <c r="K13" t="n">
-        <v>2.331506890124938</v>
-      </c>
-      <c r="L13" t="n">
-        <v>348.3119775218378</v>
-      </c>
-      <c r="M13" t="n">
-        <v>11.41428571428571</v>
-      </c>
-      <c r="N13" t="n">
-        <v>26.61248578871179</v>
+        <v>36.08310990431995</v>
       </c>
     </row>
     <row r="14">
@@ -1073,34 +950,25 @@
         <v>2.34966598409663</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6508457348060288</v>
+        <v>7</v>
       </c>
       <c r="F14" t="n">
-        <v>119.563195280721</v>
+        <v>76</v>
       </c>
       <c r="G14" t="n">
-        <v>2.490899901681688</v>
+        <v>184.2890769188558</v>
       </c>
       <c r="H14" t="n">
-        <v>39</v>
+        <v>2.424856275248102</v>
       </c>
       <c r="I14" t="n">
-        <v>552</v>
+        <v>42.77316843133559</v>
       </c>
       <c r="J14" t="n">
-        <v>1250.241120615481</v>
+        <v>10.85714285714286</v>
       </c>
       <c r="K14" t="n">
-        <v>2.264929566332394</v>
-      </c>
-      <c r="L14" t="n">
-        <v>309.4523007119865</v>
-      </c>
-      <c r="M14" t="n">
-        <v>14.15384615384615</v>
-      </c>
-      <c r="N14" t="n">
-        <v>32.05746463116619</v>
+        <v>26.32701098840797</v>
       </c>
     </row>
     <row r="15">
@@ -1119,34 +987,25 @@
         <v>2.351022852584124</v>
       </c>
       <c r="E15" t="n">
-        <v>0.4978830319103847</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
-        <v>110.8372429491116</v>
+        <v>185</v>
       </c>
       <c r="G15" t="n">
-        <v>2.131485441329069</v>
+        <v>399.1579717626575</v>
       </c>
       <c r="H15" t="n">
-        <v>59</v>
+        <v>2.157610658176527</v>
       </c>
       <c r="I15" t="n">
-        <v>1004</v>
+        <v>51.76314937262092</v>
       </c>
       <c r="J15" t="n">
-        <v>2207.906948624435</v>
+        <v>14.23076923076923</v>
       </c>
       <c r="K15" t="n">
-        <v>2.199110506598043</v>
-      </c>
-      <c r="L15" t="n">
-        <v>180.5144465708265</v>
-      </c>
-      <c r="M15" t="n">
-        <v>17.01694915254237</v>
-      </c>
-      <c r="N15" t="n">
-        <v>37.4221516716006</v>
+        <v>30.70445936635827</v>
       </c>
     </row>
     <row r="16">
@@ -1165,34 +1024,25 @@
         <v>2.754348335711019</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4446141825778798</v>
+        <v>12</v>
       </c>
       <c r="F16" t="n">
-        <v>170.3525774218905</v>
+        <v>153</v>
       </c>
       <c r="G16" t="n">
-        <v>2.399332076364655</v>
+        <v>353.8068374770822</v>
       </c>
       <c r="H16" t="n">
-        <v>40</v>
+        <v>2.312462990046289</v>
       </c>
       <c r="I16" t="n">
-        <v>523</v>
+        <v>48.09844779794895</v>
       </c>
       <c r="J16" t="n">
-        <v>1242.09511128854</v>
+        <v>12.75</v>
       </c>
       <c r="K16" t="n">
-        <v>2.374942851412123</v>
-      </c>
-      <c r="L16" t="n">
-        <v>305.0175585979932</v>
-      </c>
-      <c r="M16" t="n">
-        <v>13.075</v>
-      </c>
-      <c r="N16" t="n">
-        <v>31.0523777822135</v>
+        <v>29.48390312309019</v>
       </c>
     </row>
     <row r="17">
@@ -1211,34 +1061,25 @@
         <v>2.565965817446667</v>
       </c>
       <c r="E17" t="n">
-        <v>0.3698185250734031</v>
+        <v>11</v>
       </c>
       <c r="F17" t="n">
-        <v>114.4855624144193</v>
+        <v>182</v>
       </c>
       <c r="G17" t="n">
-        <v>2.385115883633736</v>
+        <v>432.9353910649194</v>
       </c>
       <c r="H17" t="n">
-        <v>50</v>
+        <v>2.378765884972085</v>
       </c>
       <c r="I17" t="n">
-        <v>589</v>
+        <v>17.92410270114178</v>
       </c>
       <c r="J17" t="n">
-        <v>1397.422827341259</v>
+        <v>16.54545454545455</v>
       </c>
       <c r="K17" t="n">
-        <v>2.372534511615041</v>
-      </c>
-      <c r="L17" t="n">
-        <v>72.00773273193936</v>
-      </c>
-      <c r="M17" t="n">
-        <v>11.78</v>
-      </c>
-      <c r="N17" t="n">
-        <v>27.94845654682519</v>
+        <v>39.35776282408359</v>
       </c>
     </row>
     <row r="18">
@@ -1257,34 +1098,25 @@
         <v>2.294025094095323</v>
       </c>
       <c r="E18" t="n">
-        <v>0.463546151402067</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
-        <v>92.66167265389281</v>
+        <v>114</v>
       </c>
       <c r="G18" t="n">
-        <v>2.438465069839284</v>
+        <v>269.4248548554322</v>
       </c>
       <c r="H18" t="n">
-        <v>44</v>
+        <v>2.363375919784493</v>
       </c>
       <c r="I18" t="n">
-        <v>555</v>
+        <v>42.90037998403457</v>
       </c>
       <c r="J18" t="n">
-        <v>1289.625561655395</v>
+        <v>12.66666666666667</v>
       </c>
       <c r="K18" t="n">
-        <v>2.323649660640352</v>
-      </c>
-      <c r="L18" t="n">
-        <v>334.9648021930407</v>
-      </c>
-      <c r="M18" t="n">
-        <v>12.61363636363636</v>
-      </c>
-      <c r="N18" t="n">
-        <v>29.30967185580444</v>
+        <v>29.93609498393691</v>
       </c>
     </row>
     <row r="19">
@@ -1303,34 +1135,25 @@
         <v>2.401745082237063</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2346917793355788</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
-        <v>49.83571013535231</v>
+        <v>125</v>
       </c>
       <c r="G19" t="n">
-        <v>2.373129054064396</v>
+        <v>300.2682947973356</v>
       </c>
       <c r="H19" t="n">
-        <v>50</v>
+        <v>2.402146358378685</v>
       </c>
       <c r="I19" t="n">
-        <v>579</v>
+        <v>43.82407600197941</v>
       </c>
       <c r="J19" t="n">
-        <v>1370.651738714831</v>
+        <v>17.85714285714286</v>
       </c>
       <c r="K19" t="n">
-        <v>2.367274160129242</v>
-      </c>
-      <c r="L19" t="n">
-        <v>245.932193569547</v>
-      </c>
-      <c r="M19" t="n">
-        <v>11.58</v>
-      </c>
-      <c r="N19" t="n">
-        <v>27.41303477429663</v>
+        <v>42.89547068533365</v>
       </c>
     </row>
     <row r="20">
@@ -1349,34 +1172,25 @@
         <v>2.26150077319828</v>
       </c>
       <c r="E20" t="n">
-        <v>0.3756761788330737</v>
+        <v>11</v>
       </c>
       <c r="F20" t="n">
-        <v>153.9261890645267</v>
+        <v>290</v>
       </c>
       <c r="G20" t="n">
-        <v>2.167974493866573</v>
+        <v>582.5501621153483</v>
       </c>
       <c r="H20" t="n">
-        <v>70</v>
+        <v>2.008793662466718</v>
       </c>
       <c r="I20" t="n">
-        <v>1959</v>
+        <v>57.91993469311435</v>
       </c>
       <c r="J20" t="n">
-        <v>3843.182039955613</v>
+        <v>26.36363636363636</v>
       </c>
       <c r="K20" t="n">
-        <v>1.961808085735382</v>
-      </c>
-      <c r="L20" t="n">
-        <v>461.797962247989</v>
-      </c>
-      <c r="M20" t="n">
-        <v>27.98571428571428</v>
-      </c>
-      <c r="N20" t="n">
-        <v>54.90260057079447</v>
+        <v>52.95910564684984</v>
       </c>
     </row>
     <row r="21">
@@ -1395,34 +1209,25 @@
         <v>2.51067903103221</v>
       </c>
       <c r="E21" t="n">
-        <v>0.94361702745566</v>
+        <v>18</v>
       </c>
       <c r="F21" t="n">
-        <v>550.3559605659048</v>
+        <v>214</v>
       </c>
       <c r="G21" t="n">
-        <v>2.264839343892612</v>
+        <v>485.4137362459945</v>
       </c>
       <c r="H21" t="n">
-        <v>63</v>
+        <v>2.268288487130816</v>
       </c>
       <c r="I21" t="n">
-        <v>845</v>
+        <v>33.82506856908752</v>
       </c>
       <c r="J21" t="n">
-        <v>1843.8262042814</v>
+        <v>11.88888888888889</v>
       </c>
       <c r="K21" t="n">
-        <v>2.182042845303432</v>
-      </c>
-      <c r="L21" t="n">
-        <v>104.6695334186038</v>
-      </c>
-      <c r="M21" t="n">
-        <v>13.41269841269841</v>
-      </c>
-      <c r="N21" t="n">
-        <v>29.26708260764126</v>
+        <v>26.96742979144414</v>
       </c>
     </row>
     <row r="22">
@@ -1441,34 +1246,25 @@
         <v>2.50745106090197</v>
       </c>
       <c r="E22" t="n">
-        <v>0.5749503000954396</v>
+        <v>13</v>
       </c>
       <c r="F22" t="n">
-        <v>516.0778745748296</v>
+        <v>379</v>
       </c>
       <c r="G22" t="n">
-        <v>1.911399535462332</v>
+        <v>726.0879608743425</v>
       </c>
       <c r="H22" t="n">
-        <v>89</v>
+        <v>1.91579936906159</v>
       </c>
       <c r="I22" t="n">
-        <v>2625</v>
+        <v>97.49572318175007</v>
       </c>
       <c r="J22" t="n">
-        <v>5182.938858863768</v>
+        <v>29.15384615384615</v>
       </c>
       <c r="K22" t="n">
-        <v>1.974452898614769</v>
-      </c>
-      <c r="L22" t="n">
-        <v>271.4975430328114</v>
-      </c>
-      <c r="M22" t="n">
-        <v>29.49438202247191</v>
-      </c>
-      <c r="N22" t="n">
-        <v>58.23526807712099</v>
+        <v>55.85292006725711</v>
       </c>
     </row>
     <row r="23">
@@ -1487,34 +1283,25 @@
         <v>2.230448921378274</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4373697003890192</v>
+        <v>18</v>
       </c>
       <c r="F23" t="n">
-        <v>202.2494472477925</v>
+        <v>177</v>
       </c>
       <c r="G23" t="n">
-        <v>2.592941631381955</v>
+        <v>461.7851591071527</v>
       </c>
       <c r="H23" t="n">
-        <v>87</v>
+        <v>2.608955701170354</v>
       </c>
       <c r="I23" t="n">
-        <v>890</v>
+        <v>32.7574312704863</v>
       </c>
       <c r="J23" t="n">
-        <v>2205.613878962215</v>
+        <v>9.833333333333334</v>
       </c>
       <c r="K23" t="n">
-        <v>2.478217841530579</v>
-      </c>
-      <c r="L23" t="n">
-        <v>205.1333278624767</v>
-      </c>
-      <c r="M23" t="n">
-        <v>10.22988505747126</v>
-      </c>
-      <c r="N23" t="n">
-        <v>25.35188366623236</v>
+        <v>25.65473106150849</v>
       </c>
     </row>
     <row r="24">
@@ -1533,34 +1320,25 @@
         <v>2.458184435570263</v>
       </c>
       <c r="E24" t="n">
-        <v>0.8285821510129151</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
-        <v>424.7911558764919</v>
+        <v>128</v>
       </c>
       <c r="G24" t="n">
-        <v>2.334017339980725</v>
+        <v>301.9160351380687</v>
       </c>
       <c r="H24" t="n">
-        <v>77</v>
+        <v>2.358719024516161</v>
       </c>
       <c r="I24" t="n">
-        <v>1143</v>
+        <v>36.87463065392708</v>
       </c>
       <c r="J24" t="n">
-        <v>2536.284055104018</v>
+        <v>14.22222222222222</v>
       </c>
       <c r="K24" t="n">
-        <v>2.218971176818914</v>
-      </c>
-      <c r="L24" t="n">
-        <v>157.464900010189</v>
-      </c>
-      <c r="M24" t="n">
-        <v>14.84415584415584</v>
-      </c>
-      <c r="N24" t="n">
-        <v>32.93875396238985</v>
+        <v>33.54622612645207</v>
       </c>
     </row>
     <row r="25">
@@ -1579,34 +1357,25 @@
         <v>2.608097946325279</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5607314228631708</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
-        <v>171.47714030654</v>
+        <v>114</v>
       </c>
       <c r="G25" t="n">
-        <v>2.679330317289687</v>
+        <v>298.5867054986292</v>
       </c>
       <c r="H25" t="n">
-        <v>74</v>
+        <v>2.619181627180958</v>
       </c>
       <c r="I25" t="n">
-        <v>676</v>
+        <v>64.32701390988734</v>
       </c>
       <c r="J25" t="n">
-        <v>1739.37172313272</v>
+        <v>14.25</v>
       </c>
       <c r="K25" t="n">
-        <v>2.573035093391598</v>
-      </c>
-      <c r="L25" t="n">
-        <v>281.7586870657336</v>
-      </c>
-      <c r="M25" t="n">
-        <v>9.135135135135135</v>
-      </c>
-      <c r="N25" t="n">
-        <v>23.5050232855773</v>
+        <v>37.32333818732865</v>
       </c>
     </row>
     <row r="26">
@@ -1625,34 +1394,25 @@
         <v>2.742175043223677</v>
       </c>
       <c r="E26" t="n">
-        <v>0.7525435798296588</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
-        <v>263.3670843961395</v>
+        <v>138</v>
       </c>
       <c r="G26" t="n">
-        <v>2.582030239177838</v>
+        <v>359.5880852681105</v>
       </c>
       <c r="H26" t="n">
-        <v>71</v>
+        <v>2.605710762812395</v>
       </c>
       <c r="I26" t="n">
-        <v>614</v>
+        <v>39.69263605264145</v>
       </c>
       <c r="J26" t="n">
-        <v>1589.732629405572</v>
+        <v>15.33333333333333</v>
       </c>
       <c r="K26" t="n">
-        <v>2.589141090237087</v>
-      </c>
-      <c r="L26" t="n">
-        <v>278.8083741397609</v>
-      </c>
-      <c r="M26" t="n">
-        <v>8.647887323943662</v>
-      </c>
-      <c r="N26" t="n">
-        <v>22.39060041416298</v>
+        <v>39.95423169645673</v>
       </c>
     </row>
     <row r="27">
@@ -1671,34 +1431,25 @@
         <v>2.014940349792937</v>
       </c>
       <c r="E27" t="n">
-        <v>1.235029682988136</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
-        <v>572.2183288197879</v>
+        <v>89</v>
       </c>
       <c r="G27" t="n">
-        <v>2.000763387481776</v>
+        <v>193.0327369883575</v>
       </c>
       <c r="H27" t="n">
-        <v>65</v>
+        <v>2.168907157172556</v>
       </c>
       <c r="I27" t="n">
-        <v>1291</v>
+        <v>46.40759645910545</v>
       </c>
       <c r="J27" t="n">
-        <v>2641.195233268913</v>
+        <v>22.25</v>
       </c>
       <c r="K27" t="n">
-        <v>2.045852233360893</v>
-      </c>
-      <c r="L27" t="n">
-        <v>359.544731657301</v>
-      </c>
-      <c r="M27" t="n">
-        <v>19.86153846153846</v>
-      </c>
-      <c r="N27" t="n">
-        <v>40.63377281952174</v>
+        <v>48.25818424708937</v>
       </c>
     </row>
     <row r="28">
@@ -1717,34 +1468,25 @@
         <v>2.529943401658669</v>
       </c>
       <c r="E28" t="n">
-        <v>0.4076854346659421</v>
+        <v>16</v>
       </c>
       <c r="F28" t="n">
-        <v>172.0649800683188</v>
+        <v>166</v>
       </c>
       <c r="G28" t="n">
-        <v>2.607045152550284</v>
+        <v>434.139498416731</v>
       </c>
       <c r="H28" t="n">
-        <v>98</v>
+        <v>2.61529818323332</v>
       </c>
       <c r="I28" t="n">
-        <v>1318</v>
+        <v>28.41094407672693</v>
       </c>
       <c r="J28" t="n">
-        <v>3055.025204137517</v>
+        <v>10.375</v>
       </c>
       <c r="K28" t="n">
-        <v>2.317925041075506</v>
-      </c>
-      <c r="L28" t="n">
-        <v>34.93498702456109</v>
-      </c>
-      <c r="M28" t="n">
-        <v>13.44897959183673</v>
-      </c>
-      <c r="N28" t="n">
-        <v>31.17372657283181</v>
+        <v>27.13371865104569</v>
       </c>
     </row>
     <row r="29">
@@ -1763,34 +1505,25 @@
         <v>2.308777773664721</v>
       </c>
       <c r="E29" t="n">
-        <v>0.9292847669701929</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
-        <v>532.983760700371</v>
+        <v>224</v>
       </c>
       <c r="G29" t="n">
-        <v>2.166600653253541</v>
+        <v>467.0033992005943</v>
       </c>
       <c r="H29" t="n">
-        <v>39</v>
+        <v>2.084836603574082</v>
       </c>
       <c r="I29" t="n">
-        <v>966</v>
+        <v>52.83402958668054</v>
       </c>
       <c r="J29" t="n">
-        <v>2103.478977807138</v>
+        <v>44.8</v>
       </c>
       <c r="K29" t="n">
-        <v>2.177514469779646</v>
-      </c>
-      <c r="L29" t="n">
-        <v>407.791717062463</v>
-      </c>
-      <c r="M29" t="n">
-        <v>24.76923076923077</v>
-      </c>
-      <c r="N29" t="n">
-        <v>53.93535840531123</v>
+        <v>93.40067984011887</v>
       </c>
     </row>
     <row r="30">
@@ -1809,34 +1542,25 @@
         <v>2.631950826259217</v>
       </c>
       <c r="E30" t="n">
-        <v>0.6697112784648674</v>
+        <v>9</v>
       </c>
       <c r="F30" t="n">
-        <v>207.795648975309</v>
+        <v>132</v>
       </c>
       <c r="G30" t="n">
-        <v>2.416228476457081</v>
+        <v>316.719540651989</v>
       </c>
       <c r="H30" t="n">
-        <v>61</v>
+        <v>2.399390459484765</v>
       </c>
       <c r="I30" t="n">
-        <v>870</v>
+        <v>37.53855051919437</v>
       </c>
       <c r="J30" t="n">
-        <v>2037.720032120868</v>
+        <v>14.66666666666667</v>
       </c>
       <c r="K30" t="n">
-        <v>2.342206933472262</v>
-      </c>
-      <c r="L30" t="n">
-        <v>182.6177564230693</v>
-      </c>
-      <c r="M30" t="n">
-        <v>14.26229508196721</v>
-      </c>
-      <c r="N30" t="n">
-        <v>33.40524642821095</v>
+        <v>35.19106007244321</v>
       </c>
     </row>
     <row r="31">
@@ -1855,34 +1579,25 @@
         <v>2.515078675075923</v>
       </c>
       <c r="E31" t="n">
-        <v>0.3676442172464044</v>
+        <v>5</v>
       </c>
       <c r="F31" t="n">
-        <v>80.55300569377511</v>
+        <v>96</v>
       </c>
       <c r="G31" t="n">
-        <v>2.44100017253864</v>
+        <v>238.024393070243</v>
       </c>
       <c r="H31" t="n">
-        <v>46</v>
+        <v>2.479420761148365</v>
       </c>
       <c r="I31" t="n">
-        <v>621</v>
+        <v>46.9380765567061</v>
       </c>
       <c r="J31" t="n">
-        <v>1516.013552861878</v>
+        <v>19.2</v>
       </c>
       <c r="K31" t="n">
-        <v>2.441245656782413</v>
-      </c>
-      <c r="L31" t="n">
-        <v>316.7848722415982</v>
-      </c>
-      <c r="M31" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="N31" t="n">
-        <v>32.95681636656257</v>
+        <v>47.60487861404859</v>
       </c>
     </row>
     <row r="32">
@@ -1901,34 +1616,25 @@
         <v>2.259115844185066</v>
       </c>
       <c r="E32" t="n">
-        <v>0.5527681361879657</v>
+        <v>16</v>
       </c>
       <c r="F32" t="n">
-        <v>231.257880859156</v>
+        <v>261</v>
       </c>
       <c r="G32" t="n">
-        <v>2.046529919107575</v>
+        <v>563.1874115656306</v>
       </c>
       <c r="H32" t="n">
-        <v>53</v>
+        <v>2.15780617458096</v>
       </c>
       <c r="I32" t="n">
-        <v>828</v>
+        <v>15.52480095243166</v>
       </c>
       <c r="J32" t="n">
-        <v>1852.073089665543</v>
+        <v>16.3125</v>
       </c>
       <c r="K32" t="n">
-        <v>2.236803248388337</v>
-      </c>
-      <c r="L32" t="n">
-        <v>39.35794411841812</v>
-      </c>
-      <c r="M32" t="n">
-        <v>15.62264150943396</v>
-      </c>
-      <c r="N32" t="n">
-        <v>34.94477527670836</v>
+        <v>35.19921322285191</v>
       </c>
     </row>
     <row r="33">
@@ -1947,34 +1653,25 @@
         <v>2.270911639410481</v>
       </c>
       <c r="E33" t="n">
-        <v>0.6767742280477672</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
-        <v>129.7287994659407</v>
+        <v>83</v>
       </c>
       <c r="G33" t="n">
-        <v>2.647526519713076</v>
+        <v>221.0899283402962</v>
       </c>
       <c r="H33" t="n">
-        <v>99</v>
+        <v>2.663734076389111</v>
       </c>
       <c r="I33" t="n">
-        <v>1242</v>
+        <v>49.8256656400759</v>
       </c>
       <c r="J33" t="n">
-        <v>2904.393403266755</v>
+        <v>10.375</v>
       </c>
       <c r="K33" t="n">
-        <v>2.338481001019932</v>
-      </c>
-      <c r="L33" t="n">
-        <v>286.4897824435684</v>
-      </c>
-      <c r="M33" t="n">
-        <v>12.54545454545454</v>
-      </c>
-      <c r="N33" t="n">
-        <v>29.3373071037046</v>
+        <v>27.63624104253703</v>
       </c>
     </row>
     <row r="34">
@@ -1993,34 +1690,25 @@
         <v>2.431685344686012</v>
       </c>
       <c r="E34" t="n">
-        <v>0.3956703839028865</v>
+        <v>12</v>
       </c>
       <c r="F34" t="n">
-        <v>214.8269640444023</v>
+        <v>207</v>
       </c>
       <c r="G34" t="n">
-        <v>2.148269640444023</v>
+        <v>449.160977150502</v>
       </c>
       <c r="H34" t="n">
-        <v>59</v>
+        <v>2.169859792997594</v>
       </c>
       <c r="I34" t="n">
-        <v>945</v>
+        <v>28.36066568891496</v>
       </c>
       <c r="J34" t="n">
-        <v>2109.622678057294</v>
+        <v>17.25</v>
       </c>
       <c r="K34" t="n">
-        <v>2.232404950325179</v>
-      </c>
-      <c r="L34" t="n">
-        <v>115.604344699682</v>
-      </c>
-      <c r="M34" t="n">
-        <v>16.01694915254237</v>
-      </c>
-      <c r="N34" t="n">
-        <v>35.75631657724227</v>
+        <v>37.43008142920851</v>
       </c>
     </row>
     <row r="35">
@@ -2039,34 +1727,25 @@
         <v>2.498586208817518</v>
       </c>
       <c r="E35" t="n">
-        <v>2.080101868063189</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>97.25192630101787</v>
+        <v>30</v>
       </c>
       <c r="G35" t="n">
-        <v>2.114172310891693</v>
+        <v>63.85869726719186</v>
       </c>
       <c r="H35" t="n">
-        <v>19</v>
+        <v>2.128623242239728</v>
       </c>
       <c r="I35" t="n">
-        <v>457</v>
+        <v>27.65162704298403</v>
       </c>
       <c r="J35" t="n">
-        <v>981.469877844881</v>
+        <v>30</v>
       </c>
       <c r="K35" t="n">
-        <v>2.147636494190112</v>
-      </c>
-      <c r="L35" t="n">
-        <v>311.1746092212022</v>
-      </c>
-      <c r="M35" t="n">
-        <v>24.05263157894737</v>
-      </c>
-      <c r="N35" t="n">
-        <v>51.6563093602569</v>
+        <v>63.85869726719186</v>
       </c>
     </row>
     <row r="36">
@@ -2085,34 +1764,25 @@
         <v>2.297322714205303</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9716841369454354</v>
+        <v>11</v>
       </c>
       <c r="F36" t="n">
-        <v>676.3615508790574</v>
+        <v>178</v>
       </c>
       <c r="G36" t="n">
-        <v>2.031115768405578</v>
+        <v>354.0110195956737</v>
       </c>
       <c r="H36" t="n">
-        <v>79</v>
+        <v>1.988825952784684</v>
       </c>
       <c r="I36" t="n">
-        <v>1250</v>
+        <v>79.95217296821465</v>
       </c>
       <c r="J36" t="n">
-        <v>2697.291788504207</v>
+        <v>16.18181818181818</v>
       </c>
       <c r="K36" t="n">
-        <v>2.157833430803366</v>
-      </c>
-      <c r="L36" t="n">
-        <v>415.9607987693562</v>
-      </c>
-      <c r="M36" t="n">
-        <v>15.82278481012658</v>
-      </c>
-      <c r="N36" t="n">
-        <v>34.14293403169882</v>
+        <v>32.18281996324306</v>
       </c>
     </row>
     <row r="37">
@@ -2131,34 +1801,25 @@
         <v>2.516667559099043</v>
       </c>
       <c r="E37" t="n">
-        <v>0.411275102360126</v>
+        <v>12</v>
       </c>
       <c r="F37" t="n">
-        <v>156.2025547149539</v>
+        <v>164</v>
       </c>
       <c r="G37" t="n">
-        <v>2.231465067356484</v>
+        <v>359.408679620479</v>
       </c>
       <c r="H37" t="n">
-        <v>61</v>
+        <v>2.191516339149262</v>
       </c>
       <c r="I37" t="n">
-        <v>836</v>
+        <v>33.9179378103243</v>
       </c>
       <c r="J37" t="n">
-        <v>1925.637432897514</v>
+        <v>13.66666666666667</v>
       </c>
       <c r="K37" t="n">
-        <v>2.303394058489849</v>
-      </c>
-      <c r="L37" t="n">
-        <v>85.65541141985561</v>
-      </c>
-      <c r="M37" t="n">
-        <v>13.70491803278689</v>
-      </c>
-      <c r="N37" t="n">
-        <v>31.5678267688117</v>
+        <v>29.95072330170659</v>
       </c>
     </row>
     <row r="38">
@@ -2177,34 +1838,25 @@
         <v>2.495821753385906</v>
       </c>
       <c r="E38" t="n">
-        <v>2.220009591993653</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
-        <v>632.167882416698</v>
+        <v>73</v>
       </c>
       <c r="G38" t="n">
-        <v>1.957176106553245</v>
+        <v>173.9381294316773</v>
       </c>
       <c r="H38" t="n">
-        <v>35</v>
+        <v>2.382714101803798</v>
       </c>
       <c r="I38" t="n">
-        <v>455</v>
+        <v>29.38211095496671</v>
       </c>
       <c r="J38" t="n">
-        <v>1005.539335402812</v>
+        <v>12.16666666666667</v>
       </c>
       <c r="K38" t="n">
-        <v>2.209976561324861</v>
-      </c>
-      <c r="L38" t="n">
-        <v>216.7312246975356</v>
-      </c>
-      <c r="M38" t="n">
-        <v>13</v>
-      </c>
-      <c r="N38" t="n">
-        <v>28.72969529722319</v>
+        <v>28.98968823861287</v>
       </c>
     </row>
     <row r="39">
@@ -2223,34 +1875,25 @@
         <v>2.378034322457331</v>
       </c>
       <c r="E39" t="n">
-        <v>0.8691825749138948</v>
+        <v>16</v>
       </c>
       <c r="F39" t="n">
-        <v>378.1858485210256</v>
+        <v>213</v>
       </c>
       <c r="G39" t="n">
-        <v>2.186045367173558</v>
+        <v>477.2358555058501</v>
       </c>
       <c r="H39" t="n">
-        <v>50</v>
+        <v>2.240543922562677</v>
       </c>
       <c r="I39" t="n">
-        <v>822</v>
+        <v>22.17001414021124</v>
       </c>
       <c r="J39" t="n">
-        <v>1753.041122173992</v>
+        <v>13.3125</v>
       </c>
       <c r="K39" t="n">
-        <v>2.132653433301694</v>
-      </c>
-      <c r="L39" t="n">
-        <v>108.8209306389307</v>
-      </c>
-      <c r="M39" t="n">
-        <v>16.44</v>
-      </c>
-      <c r="N39" t="n">
-        <v>35.06082244347985</v>
+        <v>29.82724096911563</v>
       </c>
     </row>
     <row r="40">
@@ -2269,34 +1912,25 @@
         <v>2.573335840066068</v>
       </c>
       <c r="E40" t="n">
-        <v>1.462380735562182</v>
+        <v>18</v>
       </c>
       <c r="F40" t="n">
-        <v>831.9242904465143</v>
+        <v>156</v>
       </c>
       <c r="G40" t="n">
-        <v>2.189274448543459</v>
+        <v>364.3777836690002</v>
       </c>
       <c r="H40" t="n">
-        <v>41</v>
+        <v>2.335755023519232</v>
       </c>
       <c r="I40" t="n">
-        <v>541</v>
+        <v>38.56870536894029</v>
       </c>
       <c r="J40" t="n">
-        <v>1194.768697702159</v>
+        <v>8.666666666666666</v>
       </c>
       <c r="K40" t="n">
-        <v>2.208444912573307</v>
-      </c>
-      <c r="L40" t="n">
-        <v>185.234703994821</v>
-      </c>
-      <c r="M40" t="n">
-        <v>13.19512195121951</v>
-      </c>
-      <c r="N40" t="n">
-        <v>29.1406999439551</v>
+        <v>20.24321020383335</v>
       </c>
     </row>
     <row r="41">
@@ -2315,34 +1949,25 @@
         <v>2.306210508167761</v>
       </c>
       <c r="E41" t="n">
-        <v>0.9602521630067394</v>
+        <v>5</v>
       </c>
       <c r="F41" t="n">
-        <v>687.8498947149689</v>
+        <v>240</v>
       </c>
       <c r="G41" t="n">
-        <v>2.169873484905264</v>
+        <v>537.6574668530518</v>
       </c>
       <c r="H41" t="n">
-        <v>52</v>
+        <v>2.240239445221049</v>
       </c>
       <c r="I41" t="n">
-        <v>1989</v>
+        <v>24.95267237615401</v>
       </c>
       <c r="J41" t="n">
-        <v>4048.195096413213</v>
+        <v>48</v>
       </c>
       <c r="K41" t="n">
-        <v>2.035291652294225</v>
-      </c>
-      <c r="L41" t="n">
-        <v>439.9362873460936</v>
-      </c>
-      <c r="M41" t="n">
-        <v>38.25</v>
-      </c>
-      <c r="N41" t="n">
-        <v>77.8499057002541</v>
+        <v>107.5314933706104</v>
       </c>
     </row>
     <row r="42">
@@ -2361,34 +1986,25 @@
         <v>2.81630759943194</v>
       </c>
       <c r="E42" t="n">
-        <v>0.4903609850451628</v>
+        <v>9</v>
       </c>
       <c r="F42" t="n">
-        <v>223.7715274810493</v>
+        <v>159</v>
       </c>
       <c r="G42" t="n">
-        <v>2.406145456785477</v>
+        <v>384.5995957769079</v>
       </c>
       <c r="H42" t="n">
-        <v>48</v>
+        <v>2.418865382244704</v>
       </c>
       <c r="I42" t="n">
-        <v>669</v>
+        <v>24.26298335429708</v>
       </c>
       <c r="J42" t="n">
-        <v>1634.345110409269</v>
+        <v>17.66666666666667</v>
       </c>
       <c r="K42" t="n">
-        <v>2.442967280133436</v>
-      </c>
-      <c r="L42" t="n">
-        <v>133.772229035461</v>
-      </c>
-      <c r="M42" t="n">
-        <v>13.9375</v>
-      </c>
-      <c r="N42" t="n">
-        <v>34.04885646685976</v>
+        <v>42.73328841965643</v>
       </c>
     </row>
     <row r="43">
@@ -2407,34 +2023,25 @@
         <v>2.338257230246255</v>
       </c>
       <c r="E43" t="n">
-        <v>0.9620822776447954</v>
+        <v>11</v>
       </c>
       <c r="F43" t="n">
-        <v>659.1789528009347</v>
+        <v>203</v>
       </c>
       <c r="G43" t="n">
-        <v>2.059934227502921</v>
+        <v>413.8625434436296</v>
       </c>
       <c r="H43" t="n">
-        <v>107</v>
+        <v>2.038731741101624</v>
       </c>
       <c r="I43" t="n">
-        <v>2503</v>
+        <v>48.98645153352845</v>
       </c>
       <c r="J43" t="n">
-        <v>4996.317775577758</v>
+        <v>18.45454545454545</v>
       </c>
       <c r="K43" t="n">
-        <v>1.996131752128549</v>
-      </c>
-      <c r="L43" t="n">
-        <v>513.7592380397675</v>
-      </c>
-      <c r="M43" t="n">
-        <v>23.39252336448598</v>
-      </c>
-      <c r="N43" t="n">
-        <v>46.69455865025942</v>
+        <v>37.62386758578452</v>
       </c>
     </row>
     <row r="44">
@@ -2453,34 +2060,25 @@
         <v>2.430236353411511</v>
       </c>
       <c r="E44" t="n">
-        <v>1.098338189042889</v>
+        <v>7</v>
       </c>
       <c r="F44" t="n">
-        <v>365.0275651199829</v>
+        <v>79</v>
       </c>
       <c r="G44" t="n">
-        <v>2.253256574814709</v>
+        <v>184.5802731800765</v>
       </c>
       <c r="H44" t="n">
-        <v>37</v>
+        <v>2.336459154178184</v>
       </c>
       <c r="I44" t="n">
-        <v>519</v>
+        <v>42.44336930754172</v>
       </c>
       <c r="J44" t="n">
-        <v>1171.285980093306</v>
+        <v>11.28571428571429</v>
       </c>
       <c r="K44" t="n">
-        <v>2.256813063763595</v>
-      </c>
-      <c r="L44" t="n">
-        <v>311.2664186114233</v>
-      </c>
-      <c r="M44" t="n">
-        <v>14.02702702702703</v>
-      </c>
-      <c r="N44" t="n">
-        <v>31.65637784035962</v>
+        <v>26.36861045429665</v>
       </c>
     </row>
     <row r="45">
@@ -2499,34 +2097,25 @@
         <v>2.310693312343361</v>
       </c>
       <c r="E45" t="n">
-        <v>1.784378809176166</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
-        <v>321.3300583118495</v>
+        <v>46</v>
       </c>
       <c r="G45" t="n">
-        <v>2.114013541525326</v>
+        <v>106.4053387310746</v>
       </c>
       <c r="H45" t="n">
-        <v>58</v>
+        <v>2.313159537632056</v>
       </c>
       <c r="I45" t="n">
-        <v>932</v>
+        <v>14.12685491780428</v>
       </c>
       <c r="J45" t="n">
-        <v>2001.96408699926</v>
+        <v>15.33333333333333</v>
       </c>
       <c r="K45" t="n">
-        <v>2.1480301362653</v>
-      </c>
-      <c r="L45" t="n">
-        <v>368.9425077030044</v>
-      </c>
-      <c r="M45" t="n">
-        <v>16.06896551724138</v>
-      </c>
-      <c r="N45" t="n">
-        <v>34.51662218964241</v>
+        <v>35.46844624369153</v>
       </c>
     </row>
     <row r="46">
@@ -2545,34 +2134,25 @@
         <v>2.367914738793753</v>
       </c>
       <c r="E46" t="n">
-        <v>1.118826625063243</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>331.1531720576009</v>
+        <v>164</v>
       </c>
       <c r="G46" t="n">
-        <v>2.178639289852637</v>
+        <v>375.317239810031</v>
       </c>
       <c r="H46" t="n">
-        <v>57</v>
+        <v>2.288519754939213</v>
       </c>
       <c r="I46" t="n">
-        <v>1713</v>
+        <v>61.69682540182696</v>
       </c>
       <c r="J46" t="n">
-        <v>3566.844787032365</v>
+        <v>23.42857142857143</v>
       </c>
       <c r="K46" t="n">
-        <v>2.082221124945923</v>
-      </c>
-      <c r="L46" t="n">
-        <v>410.458608163912</v>
-      </c>
-      <c r="M46" t="n">
-        <v>30.05263157894737</v>
-      </c>
-      <c r="N46" t="n">
-        <v>62.57622433390114</v>
+        <v>53.61674854429014</v>
       </c>
     </row>
     <row r="47">
@@ -2591,34 +2171,25 @@
         <v>2.370142847051102</v>
       </c>
       <c r="E47" t="n">
-        <v>0.4150455121639237</v>
+        <v>12</v>
       </c>
       <c r="F47" t="n">
-        <v>117.5156386939096</v>
+        <v>166</v>
       </c>
       <c r="G47" t="n">
-        <v>2.350312773878192</v>
+        <v>401.4342864564599</v>
       </c>
       <c r="H47" t="n">
-        <v>50</v>
+        <v>2.418278834075059</v>
       </c>
       <c r="I47" t="n">
-        <v>601</v>
+        <v>8.07994375662248</v>
       </c>
       <c r="J47" t="n">
-        <v>1421.318446040191</v>
+        <v>13.83333333333333</v>
       </c>
       <c r="K47" t="n">
-        <v>2.364922539168371</v>
-      </c>
-      <c r="L47" t="n">
-        <v>172.5631473108476</v>
-      </c>
-      <c r="M47" t="n">
-        <v>12.02</v>
-      </c>
-      <c r="N47" t="n">
-        <v>28.42636892080382</v>
+        <v>33.45285720470499</v>
       </c>
     </row>
     <row r="48">
@@ -2637,34 +2208,25 @@
         <v>2.363235804483694</v>
       </c>
       <c r="E48" t="n">
-        <v>0.401326677359964</v>
+        <v>8</v>
       </c>
       <c r="F48" t="n">
-        <v>123.3847183208121</v>
+        <v>125</v>
       </c>
       <c r="G48" t="n">
-        <v>2.372783044631002</v>
+        <v>297.6006166798478</v>
       </c>
       <c r="H48" t="n">
-        <v>74</v>
+        <v>2.380804933438783</v>
       </c>
       <c r="I48" t="n">
-        <v>884</v>
+        <v>40.4592116947352</v>
       </c>
       <c r="J48" t="n">
-        <v>2037.210930805215</v>
+        <v>15.625</v>
       </c>
       <c r="K48" t="n">
-        <v>2.304537252042099</v>
-      </c>
-      <c r="L48" t="n">
-        <v>140.6011851863458</v>
-      </c>
-      <c r="M48" t="n">
-        <v>11.94594594594595</v>
-      </c>
-      <c r="N48" t="n">
-        <v>27.52987744331372</v>
+        <v>37.20007708498098</v>
       </c>
     </row>
     <row r="49">
@@ -2683,34 +2245,25 @@
         <v>2.636788689034375</v>
       </c>
       <c r="E49" t="n">
-        <v>0.6255401778823841</v>
+        <v>12</v>
       </c>
       <c r="F49" t="n">
-        <v>230.8591922155824</v>
+        <v>163</v>
       </c>
       <c r="G49" t="n">
-        <v>2.593923508040252</v>
+        <v>406.4681105236265</v>
       </c>
       <c r="H49" t="n">
-        <v>41</v>
+        <v>2.4936693897155</v>
       </c>
       <c r="I49" t="n">
-        <v>586</v>
+        <v>18.90623953518588</v>
       </c>
       <c r="J49" t="n">
-        <v>1440.44650972633</v>
+        <v>13.58333333333333</v>
       </c>
       <c r="K49" t="n">
-        <v>2.458099845949368</v>
-      </c>
-      <c r="L49" t="n">
-        <v>217.2215600632617</v>
-      </c>
-      <c r="M49" t="n">
-        <v>14.29268292682927</v>
-      </c>
-      <c r="N49" t="n">
-        <v>35.13284170064219</v>
+        <v>33.87234254363554</v>
       </c>
     </row>
     <row r="50">
@@ -2729,34 +2282,25 @@
         <v>2.574147064150723</v>
       </c>
       <c r="E50" t="n">
-        <v>0.4863184604028305</v>
+        <v>11</v>
       </c>
       <c r="F50" t="n">
-        <v>204.2559729706853</v>
+        <v>166</v>
       </c>
       <c r="G50" t="n">
-        <v>2.347769804260751</v>
+        <v>400.3663215064456</v>
       </c>
       <c r="H50" t="n">
-        <v>61</v>
+        <v>2.411845310279793</v>
       </c>
       <c r="I50" t="n">
-        <v>811</v>
+        <v>16.58652156047341</v>
       </c>
       <c r="J50" t="n">
-        <v>1946.623241193609</v>
+        <v>15.09090909090909</v>
       </c>
       <c r="K50" t="n">
-        <v>2.400275266576584</v>
-      </c>
-      <c r="L50" t="n">
-        <v>230.5944743260335</v>
-      </c>
-      <c r="M50" t="n">
-        <v>13.29508196721311</v>
-      </c>
-      <c r="N50" t="n">
-        <v>31.91185641300999</v>
+        <v>36.39693831876778</v>
       </c>
     </row>
     <row r="51">
@@ -2775,34 +2319,25 @@
         <v>2.313656346618032</v>
       </c>
       <c r="E51" t="n">
-        <v>0.5008377575646211</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
-        <v>142.9243383099806</v>
+        <v>96</v>
       </c>
       <c r="G51" t="n">
-        <v>2.507444531754045</v>
+        <v>240.2751247569752</v>
       </c>
       <c r="H51" t="n">
-        <v>33</v>
+        <v>2.502865882885158</v>
       </c>
       <c r="I51" t="n">
-        <v>441</v>
+        <v>44.49385455754018</v>
       </c>
       <c r="J51" t="n">
-        <v>1089.560216915785</v>
+        <v>13.71428571428571</v>
       </c>
       <c r="K51" t="n">
-        <v>2.470658088244409</v>
-      </c>
-      <c r="L51" t="n">
-        <v>321.3594910246152</v>
-      </c>
-      <c r="M51" t="n">
-        <v>13.36363636363636</v>
-      </c>
-      <c r="N51" t="n">
-        <v>33.01697627017529</v>
+        <v>34.32501782242502</v>
       </c>
     </row>
     <row r="52">
@@ -2821,34 +2356,25 @@
         <v>2.368472838440362</v>
       </c>
       <c r="E52" t="n">
-        <v>0.4692496331279359</v>
+        <v>8</v>
       </c>
       <c r="F52" t="n">
-        <v>78.83506540192295</v>
+        <v>104</v>
       </c>
       <c r="G52" t="n">
-        <v>2.252430440054941</v>
+        <v>240.4599572477528</v>
       </c>
       <c r="H52" t="n">
-        <v>40</v>
+        <v>2.312114973536085</v>
       </c>
       <c r="I52" t="n">
-        <v>664</v>
+        <v>54.46254141508503</v>
       </c>
       <c r="J52" t="n">
-        <v>1499.237596421503</v>
+        <v>13</v>
       </c>
       <c r="K52" t="n">
-        <v>2.257887946417927</v>
-      </c>
-      <c r="L52" t="n">
-        <v>339.3416057354304</v>
-      </c>
-      <c r="M52" t="n">
-        <v>16.6</v>
-      </c>
-      <c r="N52" t="n">
-        <v>37.48093991053759</v>
+        <v>30.0574946559691</v>
       </c>
     </row>
     <row r="53">
@@ -2867,34 +2393,25 @@
         <v>2.60788374435699</v>
       </c>
       <c r="E53" t="n">
-        <v>0.7596873314374303</v>
+        <v>19</v>
       </c>
       <c r="F53" t="n">
-        <v>347.0229169434498</v>
+        <v>164</v>
       </c>
       <c r="G53" t="n">
-        <v>2.533013992287955</v>
+        <v>420.3689052950979</v>
       </c>
       <c r="H53" t="n">
-        <v>81</v>
+        <v>2.563225032287182</v>
       </c>
       <c r="I53" t="n">
-        <v>767</v>
+        <v>20.86239739677138</v>
       </c>
       <c r="J53" t="n">
-        <v>1948.58651828279</v>
+        <v>8.631578947368421</v>
       </c>
       <c r="K53" t="n">
-        <v>2.540530010798944</v>
-      </c>
-      <c r="L53" t="n">
-        <v>253.3514730712225</v>
-      </c>
-      <c r="M53" t="n">
-        <v>9.469135802469136</v>
-      </c>
-      <c r="N53" t="n">
-        <v>24.05662368250358</v>
+        <v>22.12467922605778</v>
       </c>
     </row>
     <row r="54">
@@ -2913,34 +2430,25 @@
         <v>2.156246190397344</v>
       </c>
       <c r="E54" t="n">
-        <v>0.317132989936344</v>
+        <v>19</v>
       </c>
       <c r="F54" t="n">
-        <v>85.42552932600675</v>
+        <v>222</v>
       </c>
       <c r="G54" t="n">
-        <v>2.24804024542123</v>
+        <v>520.7683660602818</v>
       </c>
       <c r="H54" t="n">
-        <v>47</v>
+        <v>2.34580345072199</v>
       </c>
       <c r="I54" t="n">
-        <v>579</v>
+        <v>9.764576593957809</v>
       </c>
       <c r="J54" t="n">
-        <v>1380.200396006905</v>
+        <v>11.68421052631579</v>
       </c>
       <c r="K54" t="n">
-        <v>2.383765796212271</v>
-      </c>
-      <c r="L54" t="n">
-        <v>118.1492179718786</v>
-      </c>
-      <c r="M54" t="n">
-        <v>12.31914893617021</v>
-      </c>
-      <c r="N54" t="n">
-        <v>29.36596587248734</v>
+        <v>27.40886137159378</v>
       </c>
     </row>
     <row r="55">
@@ -2959,34 +2467,25 @@
         <v>2.595606434865603</v>
       </c>
       <c r="E55" t="n">
-        <v>0.3947364401718058</v>
+        <v>17</v>
       </c>
       <c r="F55" t="n">
-        <v>126.7627327151366</v>
+        <v>210</v>
       </c>
       <c r="G55" t="n">
-        <v>2.437744859906473</v>
+        <v>498.1348163509213</v>
       </c>
       <c r="H55" t="n">
-        <v>56</v>
+        <v>2.372070554052006</v>
       </c>
       <c r="I55" t="n">
-        <v>687</v>
+        <v>15.64561794580339</v>
       </c>
       <c r="J55" t="n">
-        <v>1630.806630088085</v>
+        <v>12.35294117647059</v>
       </c>
       <c r="K55" t="n">
-        <v>2.373808777420793</v>
-      </c>
-      <c r="L55" t="n">
-        <v>84.82974351554248</v>
-      </c>
-      <c r="M55" t="n">
-        <v>12.26785714285714</v>
-      </c>
-      <c r="N55" t="n">
-        <v>29.12154696585866</v>
+        <v>29.30204802064243</v>
       </c>
     </row>
     <row r="56">
@@ -3005,34 +2504,25 @@
         <v>2.654465333520146</v>
       </c>
       <c r="E56" t="n">
-        <v>0.2683919616975327</v>
+        <v>13</v>
       </c>
       <c r="F56" t="n">
-        <v>55.59517813142384</v>
+        <v>204</v>
       </c>
       <c r="G56" t="n">
-        <v>2.417181657887993</v>
+        <v>485.5528668098984</v>
       </c>
       <c r="H56" t="n">
-        <v>56</v>
+        <v>2.380161111813228</v>
       </c>
       <c r="I56" t="n">
-        <v>692</v>
+        <v>13.48039422874664</v>
       </c>
       <c r="J56" t="n">
-        <v>1637.345496382653</v>
+        <v>15.69230769230769</v>
       </c>
       <c r="K56" t="n">
-        <v>2.366106208645452</v>
-      </c>
-      <c r="L56" t="n">
-        <v>80.70116250364153</v>
-      </c>
-      <c r="M56" t="n">
-        <v>12.35714285714286</v>
-      </c>
-      <c r="N56" t="n">
-        <v>29.23831243540451</v>
+        <v>37.35022052383834</v>
       </c>
     </row>
     <row r="57">
@@ -3051,34 +2541,25 @@
         <v>2.554852434372055</v>
       </c>
       <c r="E57" t="n">
-        <v>0.558448135564635</v>
+        <v>18</v>
       </c>
       <c r="F57" t="n">
-        <v>151.4225094965423</v>
+        <v>216</v>
       </c>
       <c r="G57" t="n">
-        <v>2.329577069177573</v>
+        <v>504.7865341695843</v>
       </c>
       <c r="H57" t="n">
-        <v>48</v>
+        <v>2.336974695229557</v>
       </c>
       <c r="I57" t="n">
-        <v>591</v>
+        <v>8.916899844350713</v>
       </c>
       <c r="J57" t="n">
-        <v>1409.161408787823</v>
+        <v>12</v>
       </c>
       <c r="K57" t="n">
-        <v>2.384367865969243</v>
-      </c>
-      <c r="L57" t="n">
-        <v>125.0633784950141</v>
-      </c>
-      <c r="M57" t="n">
-        <v>12.3125</v>
-      </c>
-      <c r="N57" t="n">
-        <v>29.3575293497463</v>
+        <v>28.04369634275469</v>
       </c>
     </row>
     <row r="58">
@@ -3097,34 +2578,25 @@
         <v>2.345569756056392</v>
       </c>
       <c r="E58" t="n">
-        <v>0.3954062487339601</v>
+        <v>7</v>
       </c>
       <c r="F58" t="n">
-        <v>157.7637653951211</v>
+        <v>197</v>
       </c>
       <c r="G58" t="n">
-        <v>1.900768257772544</v>
+        <v>374.5771002985318</v>
       </c>
       <c r="H58" t="n">
-        <v>63</v>
+        <v>1.901406600500162</v>
       </c>
       <c r="I58" t="n">
-        <v>1596</v>
+        <v>68.37217798446696</v>
       </c>
       <c r="J58" t="n">
-        <v>3172.995582710761</v>
+        <v>28.14285714285714</v>
       </c>
       <c r="K58" t="n">
-        <v>1.988092470370151</v>
-      </c>
-      <c r="L58" t="n">
-        <v>519.0542761153015</v>
-      </c>
-      <c r="M58" t="n">
-        <v>25.33333333333333</v>
-      </c>
-      <c r="N58" t="n">
-        <v>50.36500924937717</v>
+        <v>53.51101432836169</v>
       </c>
     </row>
     <row r="59">
@@ -3143,34 +2615,25 @@
         <v>2.52608069180203</v>
       </c>
       <c r="E59" t="n">
-        <v>0.7125309111023458</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
-        <v>250.9485467479132</v>
+        <v>91</v>
       </c>
       <c r="G59" t="n">
-        <v>2.389986159503935</v>
+        <v>219.6320330300736</v>
       </c>
       <c r="H59" t="n">
-        <v>52</v>
+        <v>2.413538824506303</v>
       </c>
       <c r="I59" t="n">
-        <v>798</v>
+        <v>49.42563095838155</v>
       </c>
       <c r="J59" t="n">
-        <v>1787.192708984868</v>
+        <v>15.16666666666667</v>
       </c>
       <c r="K59" t="n">
-        <v>2.239589860883294</v>
-      </c>
-      <c r="L59" t="n">
-        <v>469.6721631185994</v>
-      </c>
-      <c r="M59" t="n">
-        <v>15.34615384615385</v>
-      </c>
-      <c r="N59" t="n">
-        <v>34.36909055740131</v>
+        <v>36.6053388383456</v>
       </c>
     </row>
     <row r="60">
@@ -3189,34 +2652,25 @@
         <v>2.506234359612126</v>
       </c>
       <c r="E60" t="n">
-        <v>0.7981424727569201</v>
+        <v>13</v>
       </c>
       <c r="F60" t="n">
-        <v>419.527875464451</v>
+        <v>146</v>
       </c>
       <c r="G60" t="n">
-        <v>2.118827653860864</v>
+        <v>306.2112963277661</v>
       </c>
       <c r="H60" t="n">
-        <v>64</v>
+        <v>2.09733764608059</v>
       </c>
       <c r="I60" t="n">
-        <v>939</v>
+        <v>29.52643480015655</v>
       </c>
       <c r="J60" t="n">
-        <v>2019.344506013419</v>
+        <v>11.23076923076923</v>
       </c>
       <c r="K60" t="n">
-        <v>2.150526630472224</v>
-      </c>
-      <c r="L60" t="n">
-        <v>69.24360520010981</v>
-      </c>
-      <c r="M60" t="n">
-        <v>14.671875</v>
-      </c>
-      <c r="N60" t="n">
-        <v>31.55225790645967</v>
+        <v>23.55471510213586</v>
       </c>
     </row>
     <row r="61">
@@ -3235,34 +2689,25 @@
         <v>2.725012725341157</v>
       </c>
       <c r="E61" t="n">
-        <v>0.5401538202710744</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
-        <v>305.5208296652619</v>
+        <v>148</v>
       </c>
       <c r="G61" t="n">
-        <v>2.182291640466156</v>
+        <v>324.3886766021966</v>
       </c>
       <c r="H61" t="n">
-        <v>106</v>
+        <v>2.191815382447274</v>
       </c>
       <c r="I61" t="n">
-        <v>2041</v>
+        <v>33.24867456031346</v>
       </c>
       <c r="J61" t="n">
-        <v>4176.011308942896</v>
+        <v>29.6</v>
       </c>
       <c r="K61" t="n">
-        <v>2.046061395856392</v>
-      </c>
-      <c r="L61" t="n">
-        <v>302.4889405863709</v>
-      </c>
-      <c r="M61" t="n">
-        <v>19.25471698113208</v>
-      </c>
-      <c r="N61" t="n">
-        <v>39.39633310323487</v>
+        <v>64.87773532043931</v>
       </c>
     </row>
     <row r="62">
@@ -3281,34 +2726,25 @@
         <v>2.56925683332861</v>
       </c>
       <c r="E62" t="n">
-        <v>0.9806493324718679</v>
+        <v>8</v>
       </c>
       <c r="F62" t="n">
-        <v>373.9330728578445</v>
+        <v>164</v>
       </c>
       <c r="G62" t="n">
-        <v>2.112616230835279</v>
+        <v>349.1962311002978</v>
       </c>
       <c r="H62" t="n">
-        <v>93</v>
+        <v>2.129245311587182</v>
       </c>
       <c r="I62" t="n">
-        <v>1764</v>
+        <v>43.88677927071285</v>
       </c>
       <c r="J62" t="n">
-        <v>3586.347335199752</v>
+        <v>20.5</v>
       </c>
       <c r="K62" t="n">
-        <v>2.03307672063478</v>
-      </c>
-      <c r="L62" t="n">
-        <v>150.6297735008719</v>
-      </c>
-      <c r="M62" t="n">
-        <v>18.96774193548387</v>
-      </c>
-      <c r="N62" t="n">
-        <v>38.56287457204034</v>
+        <v>43.64952888753723</v>
       </c>
     </row>
     <row r="63">
@@ -3327,34 +2763,25 @@
         <v>2.666237095895804</v>
       </c>
       <c r="E63" t="n">
-        <v>0.9823109959739985</v>
+        <v>4</v>
       </c>
       <c r="F63" t="n">
-        <v>260.9282655081609</v>
+        <v>91</v>
       </c>
       <c r="G63" t="n">
-        <v>2.087426124065287</v>
+        <v>189.8302706813349</v>
       </c>
       <c r="H63" t="n">
-        <v>62</v>
+        <v>2.08604693056412</v>
       </c>
       <c r="I63" t="n">
-        <v>1049</v>
+        <v>25.35894892648097</v>
       </c>
       <c r="J63" t="n">
-        <v>2165.397289006254</v>
+        <v>22.75</v>
       </c>
       <c r="K63" t="n">
-        <v>2.064249083895381</v>
-      </c>
-      <c r="L63" t="n">
-        <v>130.9505279997658</v>
-      </c>
-      <c r="M63" t="n">
-        <v>16.91935483870968</v>
-      </c>
-      <c r="N63" t="n">
-        <v>34.92576272590733</v>
+        <v>47.45756767033372</v>
       </c>
     </row>
     <row r="64">
@@ -3373,34 +2800,25 @@
         <v>2.619302075875608</v>
       </c>
       <c r="E64" t="n">
-        <v>0.561475153789774</v>
+        <v>14</v>
       </c>
       <c r="F64" t="n">
-        <v>229.6654329158011</v>
+        <v>246</v>
       </c>
       <c r="G64" t="n">
-        <v>2.032437459431868</v>
+        <v>519.9686073590494</v>
       </c>
       <c r="H64" t="n">
-        <v>59</v>
+        <v>2.113693525849794</v>
       </c>
       <c r="I64" t="n">
-        <v>823</v>
+        <v>21.63051343770663</v>
       </c>
       <c r="J64" t="n">
-        <v>1889.491782053221</v>
+        <v>17.57142857142857</v>
       </c>
       <c r="K64" t="n">
-        <v>2.295858787427972</v>
-      </c>
-      <c r="L64" t="n">
-        <v>203.7190218328734</v>
-      </c>
-      <c r="M64" t="n">
-        <v>13.94915254237288</v>
-      </c>
-      <c r="N64" t="n">
-        <v>32.02528444158002</v>
+        <v>37.14061481136067</v>
       </c>
     </row>
     <row r="65">
@@ -3419,34 +2837,25 @@
         <v>2.550472957106563</v>
       </c>
       <c r="E65" t="n">
-        <v>0.4474875260820641</v>
+        <v>8</v>
       </c>
       <c r="F65" t="n">
-        <v>86.57731045850088</v>
+        <v>107</v>
       </c>
       <c r="G65" t="n">
-        <v>2.473637441671454</v>
+        <v>257.4530044146678</v>
       </c>
       <c r="H65" t="n">
-        <v>61</v>
+        <v>2.406102844996895</v>
       </c>
       <c r="I65" t="n">
-        <v>787</v>
+        <v>45.59998462481707</v>
       </c>
       <c r="J65" t="n">
-        <v>1784.000609123695</v>
+        <v>13.375</v>
       </c>
       <c r="K65" t="n">
-        <v>2.266836860385889</v>
-      </c>
-      <c r="L65" t="n">
-        <v>316.6390262778644</v>
-      </c>
-      <c r="M65" t="n">
-        <v>12.90163934426229</v>
-      </c>
-      <c r="N65" t="n">
-        <v>29.2459116249786</v>
+        <v>32.18162555183348</v>
       </c>
     </row>
     <row r="66">
@@ -3465,34 +2874,25 @@
         <v>2.36078268987328</v>
       </c>
       <c r="E66" t="n">
-        <v>0.3464606696537045</v>
+        <v>12</v>
       </c>
       <c r="F66" t="n">
-        <v>101.2861604506018</v>
+        <v>149</v>
       </c>
       <c r="G66" t="n">
-        <v>2.355492103502368</v>
+        <v>349.1583342684829</v>
       </c>
       <c r="H66" t="n">
-        <v>41</v>
+        <v>2.343344525291831</v>
       </c>
       <c r="I66" t="n">
-        <v>496</v>
+        <v>43.96688865145475</v>
       </c>
       <c r="J66" t="n">
-        <v>1175.992423975572</v>
+        <v>12.41666666666667</v>
       </c>
       <c r="K66" t="n">
-        <v>2.370952467692686</v>
-      </c>
-      <c r="L66" t="n">
-        <v>251.7178658529446</v>
-      </c>
-      <c r="M66" t="n">
-        <v>12.09756097560976</v>
-      </c>
-      <c r="N66" t="n">
-        <v>28.68274204818469</v>
+        <v>29.09652785570691</v>
       </c>
     </row>
     <row r="67">
@@ -3511,34 +2911,25 @@
         <v>2.540954808926133</v>
       </c>
       <c r="E67" t="n">
-        <v>0.9046649443333928</v>
+        <v>4</v>
       </c>
       <c r="F67" t="n">
-        <v>234.6287105324752</v>
+        <v>77</v>
       </c>
       <c r="G67" t="n">
-        <v>2.300281475808581</v>
+        <v>181.5373504556015</v>
       </c>
       <c r="H67" t="n">
-        <v>24</v>
+        <v>2.357627927994825</v>
       </c>
       <c r="I67" t="n">
-        <v>369</v>
+        <v>22.8946659017236</v>
       </c>
       <c r="J67" t="n">
-        <v>855.9098255775559</v>
+        <v>19.25</v>
       </c>
       <c r="K67" t="n">
-        <v>2.319538822703404</v>
-      </c>
-      <c r="L67" t="n">
-        <v>200.0682200730327</v>
-      </c>
-      <c r="M67" t="n">
-        <v>15.375</v>
-      </c>
-      <c r="N67" t="n">
-        <v>35.66290939906483</v>
+        <v>45.38433761390038</v>
       </c>
     </row>
     <row r="68">
@@ -3557,34 +2948,25 @@
         <v>2.567144045195657</v>
       </c>
       <c r="E68" t="n">
-        <v>0.5811551816655988</v>
+        <v>11</v>
       </c>
       <c r="F68" t="n">
-        <v>311.5088852050883</v>
+        <v>165</v>
       </c>
       <c r="G68" t="n">
-        <v>2.359915797008245</v>
+        <v>386.6514089372187</v>
       </c>
       <c r="H68" t="n">
-        <v>42</v>
+        <v>2.34334187234678</v>
       </c>
       <c r="I68" t="n">
-        <v>697</v>
+        <v>11.58237973702295</v>
       </c>
       <c r="J68" t="n">
-        <v>1552.484820053193</v>
+        <v>15</v>
       </c>
       <c r="K68" t="n">
-        <v>2.227381377407737</v>
-      </c>
-      <c r="L68" t="n">
-        <v>278.863137563303</v>
-      </c>
-      <c r="M68" t="n">
-        <v>16.59523809523809</v>
-      </c>
-      <c r="N68" t="n">
-        <v>36.96392428698078</v>
+        <v>35.15012808520169</v>
       </c>
     </row>
     <row r="69">
@@ -3603,34 +2985,25 @@
         <v>2.508798965403905</v>
       </c>
       <c r="E69" t="n">
-        <v>0.8821799657607026</v>
+        <v>11</v>
       </c>
       <c r="F69" t="n">
-        <v>297.0630854284023</v>
+        <v>181</v>
       </c>
       <c r="G69" t="n">
-        <v>2.320805354909393</v>
+        <v>424.5397737115442</v>
       </c>
       <c r="H69" t="n">
-        <v>51</v>
+        <v>2.34552361166599</v>
       </c>
       <c r="I69" t="n">
-        <v>811</v>
+        <v>26.47791819557922</v>
       </c>
       <c r="J69" t="n">
-        <v>1810.667016753323</v>
+        <v>16.45454545454545</v>
       </c>
       <c r="K69" t="n">
-        <v>2.232635039153295</v>
-      </c>
-      <c r="L69" t="n">
-        <v>179.3789136613166</v>
-      </c>
-      <c r="M69" t="n">
-        <v>15.90196078431373</v>
-      </c>
-      <c r="N69" t="n">
-        <v>35.50327483830044</v>
+        <v>38.59452488286765</v>
       </c>
     </row>
     <row r="70">
@@ -3649,34 +3022,25 @@
         <v>2.668199484198662</v>
       </c>
       <c r="E70" t="n">
-        <v>0.5324802204402374</v>
+        <v>11</v>
       </c>
       <c r="F70" t="n">
-        <v>140.0175843418868</v>
+        <v>231</v>
       </c>
       <c r="G70" t="n">
-        <v>2.333626405698113</v>
+        <v>524.4773749827443</v>
       </c>
       <c r="H70" t="n">
-        <v>56</v>
+        <v>2.270464826765127</v>
       </c>
       <c r="I70" t="n">
-        <v>901</v>
+        <v>16.03241705911163</v>
       </c>
       <c r="J70" t="n">
-        <v>2003.91331763953</v>
+        <v>21</v>
       </c>
       <c r="K70" t="n">
-        <v>2.224099131675394</v>
-      </c>
-      <c r="L70" t="n">
-        <v>100.3107840607723</v>
-      </c>
-      <c r="M70" t="n">
-        <v>16.08928571428572</v>
-      </c>
-      <c r="N70" t="n">
-        <v>35.78416638642018</v>
+        <v>47.67976136206767</v>
       </c>
     </row>
     <row r="71">
@@ -3695,34 +3059,25 @@
         <v>2.406880670049125</v>
       </c>
       <c r="E71" t="n">
-        <v>0.3385156277098283</v>
+        <v>12</v>
       </c>
       <c r="F71" t="n">
-        <v>53.3427727351815</v>
+        <v>146</v>
       </c>
       <c r="G71" t="n">
-        <v>2.319250988486152</v>
+        <v>319.0687248468229</v>
       </c>
       <c r="H71" t="n">
-        <v>46</v>
+        <v>2.185402224978239</v>
       </c>
       <c r="I71" t="n">
-        <v>612</v>
+        <v>48.43251759222436</v>
       </c>
       <c r="J71" t="n">
-        <v>1399.972025773412</v>
+        <v>12.16666666666667</v>
       </c>
       <c r="K71" t="n">
-        <v>2.287535989825837</v>
-      </c>
-      <c r="L71" t="n">
-        <v>272.640374823361</v>
-      </c>
-      <c r="M71" t="n">
-        <v>13.30434782608696</v>
-      </c>
-      <c r="N71" t="n">
-        <v>30.43417447333506</v>
+        <v>26.58906040390191</v>
       </c>
     </row>
     <row r="72">
@@ -3741,34 +3096,25 @@
         <v>2.249687427805302</v>
       </c>
       <c r="E72" t="n">
-        <v>0.4761614597418199</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
-        <v>103.539709043093</v>
+        <v>127</v>
       </c>
       <c r="G72" t="n">
-        <v>2.353175205524842</v>
+        <v>296.816982777304</v>
       </c>
       <c r="H72" t="n">
-        <v>44</v>
+        <v>2.337141596671685</v>
       </c>
       <c r="I72" t="n">
-        <v>609</v>
+        <v>30.84207043987126</v>
       </c>
       <c r="J72" t="n">
-        <v>1384.33868447951</v>
+        <v>14.11111111111111</v>
       </c>
       <c r="K72" t="n">
-        <v>2.27313412886619</v>
-      </c>
-      <c r="L72" t="n">
-        <v>284.1358281702632</v>
-      </c>
-      <c r="M72" t="n">
-        <v>13.84090909090909</v>
-      </c>
-      <c r="N72" t="n">
-        <v>31.46224282907977</v>
+        <v>32.97966475303378</v>
       </c>
     </row>
     <row r="73">
@@ -3787,34 +3133,25 @@
         <v>2.533772058384718</v>
       </c>
       <c r="E73" t="n">
-        <v>0.4668450384283998</v>
+        <v>17</v>
       </c>
       <c r="F73" t="n">
-        <v>128.3968371270981</v>
+        <v>178</v>
       </c>
       <c r="G73" t="n">
-        <v>2.517585041707806</v>
+        <v>454.2009516978043</v>
       </c>
       <c r="H73" t="n">
-        <v>92</v>
+        <v>2.551690739875305</v>
       </c>
       <c r="I73" t="n">
-        <v>1105</v>
+        <v>21.38100603984419</v>
       </c>
       <c r="J73" t="n">
-        <v>2615.397946627331</v>
+        <v>10.47058823529412</v>
       </c>
       <c r="K73" t="n">
-        <v>2.36687596979849</v>
-      </c>
-      <c r="L73" t="n">
-        <v>166.4041079847376</v>
-      </c>
-      <c r="M73" t="n">
-        <v>12.01086956521739</v>
-      </c>
-      <c r="N73" t="n">
-        <v>28.42823855029708</v>
+        <v>26.71770304104732</v>
       </c>
     </row>
     <row r="74">
@@ -3833,34 +3170,25 @@
         <v>2.395151591504542</v>
       </c>
       <c r="E74" t="n">
-        <v>0.9548531366586688</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
-        <v>333.3711061973702</v>
+        <v>105</v>
       </c>
       <c r="G74" t="n">
-        <v>2.283363741077878</v>
+        <v>254.4902577907213</v>
       </c>
       <c r="H74" t="n">
-        <v>53</v>
+        <v>2.423716740864012</v>
       </c>
       <c r="I74" t="n">
-        <v>929</v>
+        <v>51.38814439257686</v>
       </c>
       <c r="J74" t="n">
-        <v>2036.035804410129</v>
+        <v>11.66666666666667</v>
       </c>
       <c r="K74" t="n">
-        <v>2.191642415942012</v>
-      </c>
-      <c r="L74" t="n">
-        <v>417.4457651683181</v>
-      </c>
-      <c r="M74" t="n">
-        <v>17.52830188679245</v>
-      </c>
-      <c r="N74" t="n">
-        <v>38.41576989453075</v>
+        <v>28.27669531008014</v>
       </c>
     </row>
     <row r="75">
@@ -3879,34 +3207,25 @@
         <v>2.531478917042255</v>
       </c>
       <c r="E75" t="n">
-        <v>0.6759374449795127</v>
+        <v>5</v>
       </c>
       <c r="F75" t="n">
-        <v>380.1454046053139</v>
+        <v>258</v>
       </c>
       <c r="G75" t="n">
-        <v>1.845366041773368</v>
+        <v>470.3546500676437</v>
       </c>
       <c r="H75" t="n">
-        <v>51</v>
+        <v>1.823080039021875</v>
       </c>
       <c r="I75" t="n">
-        <v>1871</v>
+        <v>29.14897159611558</v>
       </c>
       <c r="J75" t="n">
-        <v>3607.425190735124</v>
+        <v>51.6</v>
       </c>
       <c r="K75" t="n">
-        <v>1.928073324818345</v>
-      </c>
-      <c r="L75" t="n">
-        <v>680.2376080989845</v>
-      </c>
-      <c r="M75" t="n">
-        <v>36.68627450980392</v>
-      </c>
-      <c r="N75" t="n">
-        <v>70.73382726931617</v>
+        <v>94.07093001352874</v>
       </c>
     </row>
     <row r="76">
@@ -3925,34 +3244,25 @@
         <v>2.505149978319906</v>
       </c>
       <c r="E76" t="n">
-        <v>0.5725563857306935</v>
+        <v>13</v>
       </c>
       <c r="F76" t="n">
-        <v>492.6399178165203</v>
+        <v>466</v>
       </c>
       <c r="G76" t="n">
-        <v>1.916886839752997</v>
+        <v>911.2585886578073</v>
       </c>
       <c r="H76" t="n">
-        <v>75</v>
+        <v>1.955490533600445</v>
       </c>
       <c r="I76" t="n">
-        <v>2348</v>
+        <v>77.1712802908301</v>
       </c>
       <c r="J76" t="n">
-        <v>4602.600334027716</v>
+        <v>35.84615384615385</v>
       </c>
       <c r="K76" t="n">
-        <v>1.960221607337187</v>
-      </c>
-      <c r="L76" t="n">
-        <v>482.3320547399832</v>
-      </c>
-      <c r="M76" t="n">
-        <v>31.30666666666667</v>
-      </c>
-      <c r="N76" t="n">
-        <v>61.36800445370287</v>
+        <v>70.09681451213902</v>
       </c>
     </row>
     <row r="77">
@@ -3971,34 +3281,25 @@
         <v>2.145507171409663</v>
       </c>
       <c r="E77" t="n">
-        <v>0.8916935024125903</v>
+        <v>5</v>
       </c>
       <c r="F77" t="n">
-        <v>196.0882173045558</v>
+        <v>88</v>
       </c>
       <c r="G77" t="n">
-        <v>2.154815574775339</v>
+        <v>187.5962095241755</v>
       </c>
       <c r="H77" t="n">
-        <v>67</v>
+        <v>2.131775108229267</v>
       </c>
       <c r="I77" t="n">
-        <v>1052</v>
+        <v>31.96242130338958</v>
       </c>
       <c r="J77" t="n">
-        <v>2295.278155224959</v>
+        <v>17.6</v>
       </c>
       <c r="K77" t="n">
-        <v>2.181823341468592</v>
-      </c>
-      <c r="L77" t="n">
-        <v>295.4690062617568</v>
-      </c>
-      <c r="M77" t="n">
-        <v>15.70149253731343</v>
-      </c>
-      <c r="N77" t="n">
-        <v>34.25788291380536</v>
+        <v>37.5192419048351</v>
       </c>
     </row>
     <row r="78">
@@ -4017,34 +3318,25 @@
         <v>2.73870130043471</v>
       </c>
       <c r="E78" t="n">
-        <v>0.8878610200726241</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
-        <v>700.6528816383816</v>
+        <v>497</v>
       </c>
       <c r="G78" t="n">
-        <v>2.001865376109662</v>
+        <v>956.1260839987749</v>
       </c>
       <c r="H78" t="n">
-        <v>59</v>
+        <v>1.923794937623289</v>
       </c>
       <c r="I78" t="n">
-        <v>2311</v>
+        <v>66.80146414626904</v>
       </c>
       <c r="J78" t="n">
-        <v>4595.095347765169</v>
+        <v>62.125</v>
       </c>
       <c r="K78" t="n">
-        <v>1.988358004225517</v>
-      </c>
-      <c r="L78" t="n">
-        <v>405.0839790724417</v>
-      </c>
-      <c r="M78" t="n">
-        <v>39.16949152542373</v>
-      </c>
-      <c r="N78" t="n">
-        <v>77.88297199601982</v>
+        <v>119.5157604998469</v>
       </c>
     </row>
     <row r="79">
@@ -4063,34 +3355,25 @@
         <v>2.301247088636211</v>
       </c>
       <c r="E79" t="n">
-        <v>0.454336555662236</v>
+        <v>14</v>
       </c>
       <c r="F79" t="n">
-        <v>81.46944787104395</v>
+        <v>176</v>
       </c>
       <c r="G79" t="n">
-        <v>2.715648262368132</v>
+        <v>456.938700723498</v>
       </c>
       <c r="H79" t="n">
-        <v>82</v>
+        <v>2.596242617747148</v>
       </c>
       <c r="I79" t="n">
-        <v>787</v>
+        <v>25.01589502157939</v>
       </c>
       <c r="J79" t="n">
-        <v>1983.48514137495</v>
+        <v>12.57142857142857</v>
       </c>
       <c r="K79" t="n">
-        <v>2.520311488405273</v>
-      </c>
-      <c r="L79" t="n">
-        <v>247.2200541622612</v>
-      </c>
-      <c r="M79" t="n">
-        <v>9.597560975609756</v>
-      </c>
-      <c r="N79" t="n">
-        <v>24.18884318749939</v>
+        <v>32.638478623107</v>
       </c>
     </row>
     <row r="80">
@@ -4109,34 +3392,25 @@
         <v>2.352568386179309</v>
       </c>
       <c r="E80" t="n">
-        <v>0.5277437603762941</v>
+        <v>11</v>
       </c>
       <c r="F80" t="n">
-        <v>183.9299166804091</v>
+        <v>187</v>
       </c>
       <c r="G80" t="n">
-        <v>2.189641865242966</v>
+        <v>390.2972043246942</v>
       </c>
       <c r="H80" t="n">
-        <v>65</v>
+        <v>2.087150825265744</v>
       </c>
       <c r="I80" t="n">
-        <v>937</v>
+        <v>52.96451544909149</v>
       </c>
       <c r="J80" t="n">
-        <v>2152.063959212097</v>
+        <v>17</v>
       </c>
       <c r="K80" t="n">
-        <v>2.296759828401384</v>
-      </c>
-      <c r="L80" t="n">
-        <v>196.7618124810548</v>
-      </c>
-      <c r="M80" t="n">
-        <v>14.41538461538462</v>
-      </c>
-      <c r="N80" t="n">
-        <v>33.10867629557072</v>
+        <v>35.48156402951766</v>
       </c>
     </row>
     <row r="81">
@@ -4155,34 +3429,21 @@
         <v>1.973127853599699</v>
       </c>
       <c r="E81" t="n">
-        <v>2.90638177831283</v>
+        <v>2</v>
       </c>
       <c r="F81" t="n">
-        <v>77.58746377793349</v>
+        <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>2.096958480484689</v>
-      </c>
-      <c r="H81" t="n">
-        <v>5</v>
-      </c>
-      <c r="I81" t="n">
-        <v>20</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
       <c r="J81" t="n">
-        <v>43.46936842755625</v>
+        <v>0</v>
       </c>
       <c r="K81" t="n">
-        <v>2.173468421377812</v>
-      </c>
-      <c r="L81" t="n">
-        <v>16.4191909382827</v>
-      </c>
-      <c r="M81" t="n">
-        <v>4</v>
-      </c>
-      <c r="N81" t="n">
-        <v>8.69387368551125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -4201,34 +3462,25 @@
         <v>2.298634783124435</v>
       </c>
       <c r="E82" t="n">
-        <v>0.5107173008236937</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
-        <v>283.1046460083572</v>
+        <v>236</v>
       </c>
       <c r="G82" t="n">
-        <v>2.112721238868338</v>
+        <v>518.4007675736152</v>
       </c>
       <c r="H82" t="n">
-        <v>47</v>
+        <v>2.196613421922098</v>
       </c>
       <c r="I82" t="n">
-        <v>1501</v>
+        <v>34.16603137904315</v>
       </c>
       <c r="J82" t="n">
-        <v>3146.938928352198</v>
+        <v>29.5</v>
       </c>
       <c r="K82" t="n">
-        <v>2.096561577849565</v>
-      </c>
-      <c r="L82" t="n">
-        <v>357.54964873461</v>
-      </c>
-      <c r="M82" t="n">
-        <v>31.93617021276596</v>
-      </c>
-      <c r="N82" t="n">
-        <v>66.95614741174889</v>
+        <v>64.8000959467019</v>
       </c>
     </row>
     <row r="83">
@@ -4247,34 +3499,25 @@
         <v>2.633670406051444</v>
       </c>
       <c r="E83" t="n">
-        <v>0.7183424235158414</v>
+        <v>16</v>
       </c>
       <c r="F83" t="n">
-        <v>364.4060496759263</v>
+        <v>206</v>
       </c>
       <c r="G83" t="n">
-        <v>2.047224998179361</v>
+        <v>446.0688699389378</v>
       </c>
       <c r="H83" t="n">
-        <v>86</v>
+        <v>2.165382863781252</v>
       </c>
       <c r="I83" t="n">
-        <v>1166</v>
+        <v>32.94596065989523</v>
       </c>
       <c r="J83" t="n">
-        <v>2640.523673418696</v>
+        <v>12.875</v>
       </c>
       <c r="K83" t="n">
-        <v>2.264600062966291</v>
-      </c>
-      <c r="L83" t="n">
-        <v>208.3449394641426</v>
-      </c>
-      <c r="M83" t="n">
-        <v>13.55813953488372</v>
-      </c>
-      <c r="N83" t="n">
-        <v>30.70376364440344</v>
+        <v>27.87930437118361</v>
       </c>
     </row>
     <row r="84">
@@ -4293,34 +3536,25 @@
         <v>2.625209525381881</v>
       </c>
       <c r="E84" t="n">
-        <v>1.401597490473213</v>
+        <v>12</v>
       </c>
       <c r="F84" t="n">
-        <v>275.629483403274</v>
+        <v>134</v>
       </c>
       <c r="G84" t="n">
-        <v>2.041699877061289</v>
+        <v>318.8624782261115</v>
       </c>
       <c r="H84" t="n">
-        <v>77</v>
+        <v>2.379570733030683</v>
       </c>
       <c r="I84" t="n">
-        <v>839</v>
+        <v>41.14239758654016</v>
       </c>
       <c r="J84" t="n">
-        <v>1966.516636078794</v>
+        <v>11.16666666666667</v>
       </c>
       <c r="K84" t="n">
-        <v>2.343881568627883</v>
-      </c>
-      <c r="L84" t="n">
-        <v>279.0632758307832</v>
-      </c>
-      <c r="M84" t="n">
-        <v>10.8961038961039</v>
-      </c>
-      <c r="N84" t="n">
-        <v>25.53917709193239</v>
+        <v>26.57187318550929</v>
       </c>
     </row>
     <row r="85">
@@ -4339,34 +3573,25 @@
         <v>2.102433705681336</v>
       </c>
       <c r="E85" t="n">
-        <v>1.281295497152117</v>
+        <v>11</v>
       </c>
       <c r="F85" t="n">
-        <v>574.9729149230561</v>
+        <v>121</v>
       </c>
       <c r="G85" t="n">
-        <v>2.046166957021552</v>
+        <v>259.1686211626609</v>
       </c>
       <c r="H85" t="n">
-        <v>92</v>
+        <v>2.141889431096371</v>
       </c>
       <c r="I85" t="n">
-        <v>1368</v>
+        <v>43.24610758329411</v>
       </c>
       <c r="J85" t="n">
-        <v>3041.802586186753</v>
+        <v>11</v>
       </c>
       <c r="K85" t="n">
-        <v>2.223539902183299</v>
-      </c>
-      <c r="L85" t="n">
-        <v>322.3665970938139</v>
-      </c>
-      <c r="M85" t="n">
-        <v>14.8695652173913</v>
-      </c>
-      <c r="N85" t="n">
-        <v>33.06307158898644</v>
+        <v>23.56078374206008</v>
       </c>
     </row>
     <row r="86">
@@ -4385,34 +3610,25 @@
         <v>2.392872745402079</v>
       </c>
       <c r="E86" t="n">
-        <v>0.9304190840719629</v>
+        <v>24</v>
       </c>
       <c r="F86" t="n">
-        <v>767.5425027938707</v>
+        <v>319</v>
       </c>
       <c r="G86" t="n">
-        <v>2.102856172038002</v>
+        <v>626.3805303326773</v>
       </c>
       <c r="H86" t="n">
-        <v>97</v>
+        <v>1.96357533019648</v>
       </c>
       <c r="I86" t="n">
-        <v>1436</v>
+        <v>56.22736897789989</v>
       </c>
       <c r="J86" t="n">
-        <v>3004.283361213994</v>
+        <v>13.29166666666667</v>
       </c>
       <c r="K86" t="n">
-        <v>2.092119332321723</v>
-      </c>
-      <c r="L86" t="n">
-        <v>295.9366150627695</v>
-      </c>
-      <c r="M86" t="n">
-        <v>14.80412371134021</v>
-      </c>
-      <c r="N86" t="n">
-        <v>30.97199341457726</v>
+        <v>26.09918876386155</v>
       </c>
     </row>
     <row r="87">
@@ -4431,34 +3647,25 @@
         <v>2.262925469331832</v>
       </c>
       <c r="E87" t="n">
-        <v>0.7577818202135864</v>
+        <v>27</v>
       </c>
       <c r="F87" t="n">
-        <v>592.1054850029985</v>
+        <v>344</v>
       </c>
       <c r="G87" t="n">
-        <v>1.967127857152819</v>
+        <v>678.8681001144789</v>
       </c>
       <c r="H87" t="n">
-        <v>103</v>
+        <v>1.973453779402555</v>
       </c>
       <c r="I87" t="n">
-        <v>1587</v>
+        <v>21.493575071622</v>
       </c>
       <c r="J87" t="n">
-        <v>3318.049923993919</v>
+        <v>12.74074074074074</v>
       </c>
       <c r="K87" t="n">
-        <v>2.090768698168821</v>
-      </c>
-      <c r="L87" t="n">
-        <v>122.1076417147759</v>
-      </c>
-      <c r="M87" t="n">
-        <v>15.40776699029126</v>
-      </c>
-      <c r="N87" t="n">
-        <v>32.2140769319798</v>
+        <v>25.14326296720292</v>
       </c>
     </row>
     <row r="88">
@@ -4477,34 +3684,25 @@
         <v>2.242541428298384</v>
       </c>
       <c r="E88" t="n">
-        <v>1.38635274067599</v>
+        <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>497.5227946346539</v>
+        <v>109</v>
       </c>
       <c r="G88" t="n">
-        <v>2.153778331751749</v>
+        <v>265.7098300565422</v>
       </c>
       <c r="H88" t="n">
-        <v>36</v>
+        <v>2.437704862904057</v>
       </c>
       <c r="I88" t="n">
-        <v>522</v>
+        <v>37.47002927126888</v>
       </c>
       <c r="J88" t="n">
-        <v>1169.700289861953</v>
+        <v>15.57142857142857</v>
       </c>
       <c r="K88" t="n">
-        <v>2.240805152992248</v>
-      </c>
-      <c r="L88" t="n">
-        <v>164.5048347637225</v>
-      </c>
-      <c r="M88" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="N88" t="n">
-        <v>32.4916747183876</v>
+        <v>37.9585471509346</v>
       </c>
     </row>
     <row r="89">
@@ -4523,34 +3721,25 @@
         <v>2.479143247978613</v>
       </c>
       <c r="E89" t="n">
-        <v>0.4779044290256231</v>
+        <v>10</v>
       </c>
       <c r="F89" t="n">
-        <v>169.9278963427226</v>
+        <v>101</v>
       </c>
       <c r="G89" t="n">
-        <v>2.574665096101858</v>
+        <v>254.4456910878118</v>
       </c>
       <c r="H89" t="n">
-        <v>66</v>
+        <v>2.519264268196156</v>
       </c>
       <c r="I89" t="n">
-        <v>1027</v>
+        <v>25.3464306937338</v>
       </c>
       <c r="J89" t="n">
-        <v>2247.114934969064</v>
+        <v>10.1</v>
       </c>
       <c r="K89" t="n">
-        <v>2.188037911362283</v>
-      </c>
-      <c r="L89" t="n">
-        <v>456.2974851453007</v>
-      </c>
-      <c r="M89" t="n">
-        <v>15.56060606060606</v>
-      </c>
-      <c r="N89" t="n">
-        <v>34.04719598437975</v>
+        <v>25.44456910878117</v>
       </c>
     </row>
     <row r="90">
@@ -4569,34 +3758,25 @@
         <v>2.23578087032756</v>
       </c>
       <c r="E90" t="n">
-        <v>0.8274475513622221</v>
+        <v>11</v>
       </c>
       <c r="F90" t="n">
-        <v>226.7532797763145</v>
+        <v>115</v>
       </c>
       <c r="G90" t="n">
-        <v>2.313808977309332</v>
+        <v>281.8965883355874</v>
       </c>
       <c r="H90" t="n">
-        <v>69</v>
+        <v>2.45127468117902</v>
       </c>
       <c r="I90" t="n">
-        <v>1142</v>
+        <v>35.1789447856132</v>
       </c>
       <c r="J90" t="n">
-        <v>2485.797628617172</v>
+        <v>10.45454545454546</v>
       </c>
       <c r="K90" t="n">
-        <v>2.176705454130623</v>
-      </c>
-      <c r="L90" t="n">
-        <v>425.5531278495353</v>
-      </c>
-      <c r="M90" t="n">
-        <v>16.55072463768116</v>
-      </c>
-      <c r="N90" t="n">
-        <v>36.02605258865466</v>
+        <v>25.62696257596249</v>
       </c>
     </row>
     <row r="91">
@@ -4615,34 +3795,25 @@
         <v>2.236537261488694</v>
       </c>
       <c r="E91" t="n">
-        <v>0.9928983073175628</v>
+        <v>10</v>
       </c>
       <c r="F91" t="n">
-        <v>707.1574362365232</v>
+        <v>194</v>
       </c>
       <c r="G91" t="n">
-        <v>1.932124142722741</v>
+        <v>385.6169859166007</v>
       </c>
       <c r="H91" t="n">
-        <v>50</v>
+        <v>1.987716422250519</v>
       </c>
       <c r="I91" t="n">
-        <v>921</v>
+        <v>50.11863975608551</v>
       </c>
       <c r="J91" t="n">
-        <v>1847.14867769216</v>
+        <v>19.4</v>
       </c>
       <c r="K91" t="n">
-        <v>2.005590312369337</v>
-      </c>
-      <c r="L91" t="n">
-        <v>139.2604861417639</v>
-      </c>
-      <c r="M91" t="n">
-        <v>18.42</v>
-      </c>
-      <c r="N91" t="n">
-        <v>36.9429735538432</v>
+        <v>38.56169859166007</v>
       </c>
     </row>
     <row r="92">
@@ -4661,34 +3832,25 @@
         <v>2.419625360887743</v>
       </c>
       <c r="E92" t="n">
-        <v>1.645569913544903</v>
+        <v>6</v>
       </c>
       <c r="F92" t="n">
-        <v>299.4168985141046</v>
+        <v>63</v>
       </c>
       <c r="G92" t="n">
-        <v>2.050800674754141</v>
+        <v>145.9908148979512</v>
       </c>
       <c r="H92" t="n">
-        <v>46</v>
+        <v>2.317314522189702</v>
       </c>
       <c r="I92" t="n">
-        <v>744</v>
+        <v>37.91314536168233</v>
       </c>
       <c r="J92" t="n">
-        <v>1530.006735105567</v>
+        <v>10.5</v>
       </c>
       <c r="K92" t="n">
-        <v>2.056460665464472</v>
-      </c>
-      <c r="L92" t="n">
-        <v>222.9465671680271</v>
-      </c>
-      <c r="M92" t="n">
-        <v>16.17391304347826</v>
-      </c>
-      <c r="N92" t="n">
-        <v>33.26101598055581</v>
+        <v>24.33180248299187</v>
       </c>
     </row>
     <row r="93">
@@ -4707,34 +3869,25 @@
         <v>2.485153349903652</v>
       </c>
       <c r="E93" t="n">
-        <v>0.3926448022899315</v>
+        <v>5</v>
       </c>
       <c r="F93" t="n">
-        <v>250.0624105917712</v>
+        <v>241</v>
       </c>
       <c r="G93" t="n">
-        <v>1.852314152531638</v>
+        <v>444.8911269587631</v>
       </c>
       <c r="H93" t="n">
-        <v>48</v>
+        <v>1.846021273687814</v>
       </c>
       <c r="I93" t="n">
-        <v>1359</v>
+        <v>73.81619838264645</v>
       </c>
       <c r="J93" t="n">
-        <v>2671.334052169756</v>
+        <v>48.2</v>
       </c>
       <c r="K93" t="n">
-        <v>1.965661554208797</v>
-      </c>
-      <c r="L93" t="n">
-        <v>609.4104860229369</v>
-      </c>
-      <c r="M93" t="n">
-        <v>28.3125</v>
-      </c>
-      <c r="N93" t="n">
-        <v>55.65279275353657</v>
+        <v>88.97822539175262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>